<commit_message>
Correctamente usando ultras en los 0.5 (y en todos lados
</commit_message>
<xml_diff>
--- a/Code/Limpio/Excels/preprocessed/preprocessed_mm_modelo MM - TALCA 28.12_v4.xlsx
+++ b/Code/Limpio/Excels/preprocessed/preprocessed_mm_modelo MM - TALCA 28.12_v4.xlsx
@@ -18,7 +18,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="700" uniqueCount="290">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="732" uniqueCount="295">
   <si>
     <t>Unnamed: 0</t>
   </si>
@@ -776,6 +776,15 @@
     <t>12/05/2022</t>
   </si>
   <si>
+    <t>16/02/2022</t>
+  </si>
+  <si>
+    <t>20/01/2021</t>
+  </si>
+  <si>
+    <t>03/11/2020</t>
+  </si>
+  <si>
     <t>13/11/2009</t>
   </si>
   <si>
@@ -803,6 +812,9 @@
     <t>R315</t>
   </si>
   <si>
+    <t>R800</t>
+  </si>
+  <si>
     <t>B-25</t>
   </si>
   <si>
@@ -818,6 +830,9 @@
     <t>C-25</t>
   </si>
   <si>
+    <t>ULTRA</t>
+  </si>
+  <si>
     <t>C</t>
   </si>
   <si>
@@ -827,9 +842,6 @@
     <t>AB-13/19</t>
   </si>
   <si>
-    <t>ULTRA</t>
-  </si>
-  <si>
     <t>C-19</t>
   </si>
   <si>
@@ -840,6 +852,9 @@
   </si>
   <si>
     <t>19</t>
+  </si>
+  <si>
+    <t>38</t>
   </si>
   <si>
     <t>N_medidores</t>
@@ -4403,7 +4418,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:AV21"/>
+  <dimension ref="A1:AV24"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -4566,7 +4581,7 @@
         <v>238</v>
       </c>
       <c r="D2" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E2">
         <v>60274432</v>
@@ -4578,22 +4593,22 @@
         <v>121</v>
       </c>
       <c r="H2" t="s">
+        <v>265</v>
+      </c>
+      <c r="I2" t="s">
         <v>261</v>
       </c>
-      <c r="I2" t="s">
-        <v>258</v>
-      </c>
       <c r="J2">
         <v>1</v>
       </c>
       <c r="K2" t="s">
-        <v>267</v>
+        <v>272</v>
       </c>
       <c r="L2">
         <v>2.271232876712329</v>
       </c>
       <c r="M2" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="N2">
         <v>0.007117292039837499</v>
@@ -4643,6 +4658,54 @@
       <c r="AC2">
         <v>-0.01509139912581338</v>
       </c>
+      <c r="AD2">
+        <v>-0.02</v>
+      </c>
+      <c r="AE2">
+        <v>-0.02</v>
+      </c>
+      <c r="AF2">
+        <v>-0.02</v>
+      </c>
+      <c r="AG2">
+        <v>-0.02</v>
+      </c>
+      <c r="AH2">
+        <v>-0.02</v>
+      </c>
+      <c r="AI2">
+        <v>-0.02</v>
+      </c>
+      <c r="AJ2">
+        <v>-0.02</v>
+      </c>
+      <c r="AK2">
+        <v>-0.02</v>
+      </c>
+      <c r="AL2">
+        <v>-0.02</v>
+      </c>
+      <c r="AM2">
+        <v>-0.02</v>
+      </c>
+      <c r="AN2">
+        <v>-0.02</v>
+      </c>
+      <c r="AO2">
+        <v>-0.02</v>
+      </c>
+      <c r="AP2">
+        <v>-0.02</v>
+      </c>
+      <c r="AQ2">
+        <v>-0.02</v>
+      </c>
+      <c r="AR2">
+        <v>-0.02</v>
+      </c>
+      <c r="AS2">
+        <v>-0.02</v>
+      </c>
       <c r="AT2">
         <v>-0.09187092431953553</v>
       </c>
@@ -4650,7 +4713,7 @@
         <v>1</v>
       </c>
       <c r="AV2" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="3" spans="1:48">
@@ -4664,7 +4727,7 @@
         <v>239</v>
       </c>
       <c r="D3" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E3">
         <v>1252181</v>
@@ -4676,22 +4739,22 @@
         <v>121</v>
       </c>
       <c r="H3" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="I3" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="J3">
         <v>1</v>
       </c>
       <c r="K3" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="L3">
         <v>13.41369863013699</v>
       </c>
       <c r="M3" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="N3">
         <v>-0.04633522557134629</v>
@@ -4796,7 +4859,7 @@
         <v>1</v>
       </c>
       <c r="AV3" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="4" spans="1:48">
@@ -4810,7 +4873,7 @@
         <v>240</v>
       </c>
       <c r="D4" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E4">
         <v>60209133</v>
@@ -4822,22 +4885,22 @@
         <v>121</v>
       </c>
       <c r="H4" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="I4" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="J4">
         <v>1</v>
       </c>
       <c r="K4" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="L4">
         <v>4.794520547945205</v>
       </c>
       <c r="M4" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="N4">
         <v>-0.0221525938800527</v>
@@ -4942,7 +5005,7 @@
         <v>1</v>
       </c>
       <c r="AV4" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="5" spans="1:48">
@@ -4956,7 +5019,7 @@
         <v>241</v>
       </c>
       <c r="D5" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E5">
         <v>413560</v>
@@ -4968,22 +5031,22 @@
         <v>121</v>
       </c>
       <c r="H5" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="I5" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="L5">
         <v>15</v>
       </c>
       <c r="M5" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="N5">
         <v>-0.04896253477920987</v>
@@ -5088,7 +5151,7 @@
         <v>1</v>
       </c>
       <c r="AV5" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="6" spans="1:48">
@@ -5102,7 +5165,7 @@
         <v>242</v>
       </c>
       <c r="D6" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E6">
         <v>60177677</v>
@@ -5114,22 +5177,22 @@
         <v>121</v>
       </c>
       <c r="H6" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="I6" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="J6">
         <v>1</v>
       </c>
       <c r="K6" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="L6">
         <v>6.18082191780822</v>
       </c>
       <c r="M6" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="N6">
         <v>-0.02812248986069876</v>
@@ -5234,7 +5297,7 @@
         <v>1</v>
       </c>
       <c r="AV6" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="7" spans="1:48">
@@ -5248,7 +5311,7 @@
         <v>243</v>
       </c>
       <c r="D7" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E7">
         <v>3892942</v>
@@ -5260,22 +5323,22 @@
         <v>121</v>
       </c>
       <c r="H7" t="s">
-        <v>263</v>
+        <v>267</v>
       </c>
       <c r="I7" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="J7">
         <v>1</v>
       </c>
       <c r="K7" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="L7">
         <v>15</v>
       </c>
       <c r="M7" t="s">
-        <v>270</v>
+        <v>274</v>
       </c>
       <c r="N7">
         <v>-0.04896253477920987</v>
@@ -5380,7 +5443,7 @@
         <v>1</v>
       </c>
       <c r="AV7" t="s">
-        <v>273</v>
+        <v>277</v>
       </c>
     </row>
     <row r="8" spans="1:48">
@@ -5394,7 +5457,7 @@
         <v>244</v>
       </c>
       <c r="D8" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E8">
         <v>457415</v>
@@ -5406,22 +5469,22 @@
         <v>121</v>
       </c>
       <c r="H8" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="I8" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="J8">
         <v>1</v>
       </c>
       <c r="K8" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="L8">
         <v>15</v>
       </c>
       <c r="M8" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="N8">
         <v>-0.04896253477920987</v>
@@ -5526,7 +5589,7 @@
         <v>1</v>
       </c>
       <c r="AV8" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="9" spans="1:48">
@@ -5540,7 +5603,7 @@
         <v>245</v>
       </c>
       <c r="D9" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E9">
         <v>1310176</v>
@@ -5552,22 +5615,22 @@
         <v>121</v>
       </c>
       <c r="H9" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="I9" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="J9">
         <v>1</v>
       </c>
       <c r="K9" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="L9">
         <v>15</v>
       </c>
       <c r="M9" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="N9">
         <v>-0.04896253477920987</v>
@@ -5672,7 +5735,7 @@
         <v>1</v>
       </c>
       <c r="AV9" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="10" spans="1:48">
@@ -5686,7 +5749,7 @@
         <v>246</v>
       </c>
       <c r="D10" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E10">
         <v>406049</v>
@@ -5698,22 +5761,22 @@
         <v>121</v>
       </c>
       <c r="H10" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="I10" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="J10">
         <v>1</v>
       </c>
       <c r="K10" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="L10">
         <v>13.13698630136986</v>
       </c>
       <c r="M10" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="N10">
         <v>-0.04584525506024515</v>
@@ -5818,7 +5881,7 @@
         <v>1</v>
       </c>
       <c r="AV10" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="11" spans="1:48">
@@ -5832,7 +5895,7 @@
         <v>247</v>
       </c>
       <c r="D11" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E11">
         <v>4520541</v>
@@ -5844,22 +5907,22 @@
         <v>121</v>
       </c>
       <c r="H11" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="I11" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="J11">
         <v>1</v>
       </c>
       <c r="K11" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="L11">
         <v>15</v>
       </c>
       <c r="M11" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="N11">
         <v>-0.04896253477920987</v>
@@ -5964,7 +6027,7 @@
         <v>1</v>
       </c>
       <c r="AV11" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="12" spans="1:48">
@@ -5978,7 +6041,7 @@
         <v>248</v>
       </c>
       <c r="D12" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="E12">
         <v>1395912</v>
@@ -5990,22 +6053,22 @@
         <v>121</v>
       </c>
       <c r="H12" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="I12" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="L12">
         <v>2</v>
       </c>
       <c r="M12" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="N12">
         <v>0.01708602373512184</v>
@@ -6110,7 +6173,7 @@
         <v>1</v>
       </c>
       <c r="AV12" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="13" spans="1:48">
@@ -6124,7 +6187,7 @@
         <v>249</v>
       </c>
       <c r="D13" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="E13">
         <v>3936370</v>
@@ -6136,22 +6199,22 @@
         <v>121</v>
       </c>
       <c r="H13" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="I13" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="J13">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="L13">
         <v>1.983561643835617</v>
       </c>
       <c r="M13" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="N13">
         <v>0.01730402805126439</v>
@@ -6256,7 +6319,7 @@
         <v>1</v>
       </c>
       <c r="AV13" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="14" spans="1:48">
@@ -6270,7 +6333,7 @@
         <v>250</v>
       </c>
       <c r="D14" t="s">
-        <v>259</v>
+        <v>262</v>
       </c>
       <c r="E14">
         <v>60058696</v>
@@ -6282,22 +6345,22 @@
         <v>121</v>
       </c>
       <c r="H14" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="I14" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="J14">
         <v>1</v>
       </c>
       <c r="K14" t="s">
-        <v>265</v>
+        <v>269</v>
       </c>
       <c r="L14">
         <v>2.476712328767123</v>
       </c>
       <c r="M14" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="N14">
         <v>0.006776342712931059</v>
@@ -6347,6 +6410,54 @@
       <c r="AC14">
         <v>-0.01261484408687026</v>
       </c>
+      <c r="AD14">
+        <v>-0.02</v>
+      </c>
+      <c r="AE14">
+        <v>-0.02</v>
+      </c>
+      <c r="AF14">
+        <v>-0.02</v>
+      </c>
+      <c r="AG14">
+        <v>-0.02</v>
+      </c>
+      <c r="AH14">
+        <v>-0.02</v>
+      </c>
+      <c r="AI14">
+        <v>-0.02</v>
+      </c>
+      <c r="AJ14">
+        <v>-0.02</v>
+      </c>
+      <c r="AK14">
+        <v>-0.02</v>
+      </c>
+      <c r="AL14">
+        <v>-0.02</v>
+      </c>
+      <c r="AM14">
+        <v>-0.02</v>
+      </c>
+      <c r="AN14">
+        <v>-0.02</v>
+      </c>
+      <c r="AO14">
+        <v>-0.02</v>
+      </c>
+      <c r="AP14">
+        <v>-0.02</v>
+      </c>
+      <c r="AQ14">
+        <v>-0.02</v>
+      </c>
+      <c r="AR14">
+        <v>-0.02</v>
+      </c>
+      <c r="AS14">
+        <v>-0.02</v>
+      </c>
       <c r="AT14">
         <v>-0.127883926234053</v>
       </c>
@@ -6354,7 +6465,7 @@
         <v>1</v>
       </c>
       <c r="AV14" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
     </row>
     <row r="15" spans="1:48">
@@ -6368,7 +6479,7 @@
         <v>251</v>
       </c>
       <c r="D15" t="s">
-        <v>260</v>
+        <v>263</v>
       </c>
       <c r="E15">
         <v>4565068</v>
@@ -6380,22 +6491,22 @@
         <v>121</v>
       </c>
       <c r="H15" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="I15" t="s">
-        <v>266</v>
+        <v>271</v>
       </c>
       <c r="J15">
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="L15">
         <v>0.8849315068493151</v>
       </c>
       <c r="M15" t="s">
-        <v>264</v>
+        <v>268</v>
       </c>
       <c r="N15">
         <v>0.03862436956382281</v>
@@ -6500,402 +6611,450 @@
         <v>1</v>
       </c>
       <c r="AV15" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="16" spans="1:48">
       <c r="A16" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B16">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C16" t="s">
         <v>252</v>
       </c>
       <c r="D16" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="E16">
-        <v>1218441</v>
+        <v>345317</v>
       </c>
       <c r="F16">
-        <v>2</v>
+        <v>124</v>
       </c>
       <c r="G16" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H16" t="s">
-        <v>262</v>
+        <v>270</v>
       </c>
       <c r="I16" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="J16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K16" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="L16">
-        <v>13.38630136986301</v>
+        <v>1.117808219178082</v>
       </c>
       <c r="M16" t="s">
-        <v>264</v>
+        <v>270</v>
       </c>
       <c r="N16">
-        <v>-0.04628716665981197</v>
+        <v>-0.02</v>
       </c>
       <c r="O16">
-        <v>-0.04798509368362156</v>
+        <v>-0.02</v>
       </c>
       <c r="P16">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="Q16">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="R16">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="S16">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="T16">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="U16">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="V16">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="W16">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="X16">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="Y16">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="Z16">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="AA16">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="AB16">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="AC16">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="AD16">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AE16">
-        <v>-0.03503863675043723</v>
+        <v>-0.02</v>
       </c>
       <c r="AF16">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AG16">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AH16">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AI16">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AJ16">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AK16">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AL16">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AM16">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AN16">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AO16">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AP16">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AQ16">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AR16">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AS16">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AT16">
-        <v>0.09706730378724263</v>
+        <v>2.530612244897959</v>
       </c>
       <c r="AU16">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV16" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
     </row>
     <row r="17" spans="1:48">
       <c r="A17" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B17">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C17" t="s">
         <v>253</v>
       </c>
       <c r="D17" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="E17">
-        <v>60055924</v>
+        <v>941780</v>
       </c>
       <c r="F17">
         <v>18</v>
       </c>
       <c r="G17" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H17" t="s">
-        <v>263</v>
+        <v>270</v>
       </c>
       <c r="I17" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="J17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K17" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="L17">
-        <v>10.01369863013699</v>
+        <v>2.191780821917808</v>
       </c>
       <c r="M17" t="s">
         <v>270</v>
       </c>
       <c r="N17">
-        <v>-0.03946400935227341</v>
+        <v>-0.02</v>
       </c>
       <c r="O17">
-        <v>-0.04170725587089447</v>
+        <v>-0.02</v>
       </c>
       <c r="P17">
-        <v>-0.04374958793004801</v>
+        <v>-0.02</v>
       </c>
       <c r="Q17">
-        <v>-0.04562856661191542</v>
+        <v>-0.02</v>
       </c>
       <c r="R17">
-        <v>-0.04736839890979524</v>
+        <v>-0.02</v>
       </c>
       <c r="S17">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="T17">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="U17">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="V17">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="W17">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="X17">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="Y17">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="Z17">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="AA17">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="AB17">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="AC17">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="AD17">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AE17">
-        <v>-0.03756930381072473</v>
+        <v>-0.02</v>
       </c>
       <c r="AF17">
-        <v>-0.03927017866165177</v>
+        <v>-0.02</v>
       </c>
       <c r="AG17">
-        <v>-0.04083501116334636</v>
+        <v>-0.02</v>
       </c>
       <c r="AH17">
-        <v>-0.04228396114531983</v>
+        <v>-0.02</v>
       </c>
       <c r="AI17">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AJ17">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AK17">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AL17">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AM17">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AN17">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AO17">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AP17">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AQ17">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AR17">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AS17">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AT17">
-        <v>0.7395372742482074</v>
+        <v>0.3673469387755102</v>
       </c>
       <c r="AU17">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV17" t="s">
-        <v>273</v>
+        <v>278</v>
       </c>
     </row>
     <row r="18" spans="1:48">
       <c r="A18" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B18">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C18" t="s">
         <v>254</v>
       </c>
       <c r="D18" t="s">
-        <v>258</v>
+        <v>264</v>
       </c>
       <c r="E18">
-        <v>60144910</v>
+        <v>941731</v>
       </c>
       <c r="F18">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="G18" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="H18" t="s">
-        <v>261</v>
+        <v>270</v>
       </c>
       <c r="I18" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="J18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K18" t="s">
-        <v>267</v>
+        <v>270</v>
       </c>
       <c r="L18">
-        <v>7.317808219178082</v>
+        <v>2.405479452054795</v>
       </c>
       <c r="M18" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="N18">
-        <v>-0.006647356104413221</v>
+        <v>-0.02</v>
       </c>
       <c r="O18">
-        <v>-0.008158156386945684</v>
+        <v>-0.02</v>
       </c>
       <c r="P18">
-        <v>-0.009493379801801163</v>
+        <v>-0.02</v>
       </c>
       <c r="Q18">
-        <v>-0.01069239212509018</v>
+        <v>-0.02</v>
       </c>
       <c r="R18">
-        <v>-0.01178042952012766</v>
+        <v>-0.02</v>
       </c>
       <c r="S18">
-        <v>-0.01277892143247003</v>
+        <v>-0.02</v>
       </c>
       <c r="T18">
-        <v>-0.01369684080868297</v>
+        <v>-0.02</v>
       </c>
       <c r="U18">
-        <v>-0.01454829609654285</v>
+        <v>-0.02</v>
       </c>
       <c r="V18">
-        <v>-0.01509139912581338</v>
+        <v>-0.02</v>
       </c>
       <c r="W18">
-        <v>-0.01509139912581338</v>
+        <v>-0.02</v>
       </c>
       <c r="X18">
-        <v>-0.01509139912581338</v>
+        <v>-0.02</v>
       </c>
       <c r="Y18">
-        <v>-0.01509139912581338</v>
+        <v>-0.02</v>
       </c>
       <c r="Z18">
-        <v>-0.01509139912581338</v>
+        <v>-0.02</v>
       </c>
       <c r="AA18">
-        <v>-0.01509139912581338</v>
+        <v>-0.02</v>
       </c>
       <c r="AB18">
-        <v>-0.01509139912581338</v>
+        <v>-0.02</v>
       </c>
       <c r="AC18">
-        <v>-0.01509139912581338</v>
+        <v>-0.02</v>
+      </c>
+      <c r="AD18">
+        <v>-0.02</v>
+      </c>
+      <c r="AE18">
+        <v>-0.02</v>
+      </c>
+      <c r="AF18">
+        <v>-0.02</v>
+      </c>
+      <c r="AG18">
+        <v>-0.02</v>
+      </c>
+      <c r="AH18">
+        <v>-0.02</v>
+      </c>
+      <c r="AI18">
+        <v>-0.02</v>
+      </c>
+      <c r="AJ18">
+        <v>-0.02</v>
+      </c>
+      <c r="AK18">
+        <v>-0.02</v>
+      </c>
+      <c r="AL18">
+        <v>-0.02</v>
+      </c>
+      <c r="AM18">
+        <v>-0.02</v>
+      </c>
+      <c r="AN18">
+        <v>-0.02</v>
+      </c>
+      <c r="AO18">
+        <v>-0.02</v>
+      </c>
+      <c r="AP18">
+        <v>-0.02</v>
+      </c>
+      <c r="AQ18">
+        <v>-0.02</v>
+      </c>
+      <c r="AR18">
+        <v>-0.02</v>
+      </c>
+      <c r="AS18">
+        <v>-0.02</v>
       </c>
       <c r="AT18">
-        <v>0.2475980482608367</v>
+        <v>0.6326530612244898</v>
       </c>
       <c r="AU18">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV18" t="s">
-        <v>271</v>
+        <v>278</v>
       </c>
     </row>
     <row r="19" spans="1:48">
       <c r="A19" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B19">
         <v>13</v>
@@ -6904,40 +7063,40 @@
         <v>255</v>
       </c>
       <c r="D19" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E19">
-        <v>496678</v>
+        <v>1218441</v>
       </c>
       <c r="F19">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="G19" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="H19" t="s">
-        <v>262</v>
+        <v>266</v>
       </c>
       <c r="I19" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="J19">
         <v>1</v>
       </c>
       <c r="K19" t="s">
+        <v>273</v>
+      </c>
+      <c r="L19">
+        <v>13.38630136986301</v>
+      </c>
+      <c r="M19" t="s">
         <v>268</v>
       </c>
-      <c r="L19">
-        <v>14.62191780821918</v>
-      </c>
-      <c r="M19" t="s">
-        <v>264</v>
-      </c>
       <c r="N19">
-        <v>-0.04836247008897316</v>
+        <v>-0.04628716665981197</v>
       </c>
       <c r="O19">
-        <v>-0.04896253477920987</v>
+        <v>-0.04798509368362156</v>
       </c>
       <c r="P19">
         <v>-0.04896253477920987</v>
@@ -6985,7 +7144,7 @@
         <v>-0.0361370479186777</v>
       </c>
       <c r="AE19">
-        <v>-0.0361370479186777</v>
+        <v>-0.03503863675043723</v>
       </c>
       <c r="AF19">
         <v>-0.0361370479186777</v>
@@ -7030,69 +7189,69 @@
         <v>-0.0361370479186777</v>
       </c>
       <c r="AT19">
-        <v>0.4573823720901941</v>
+        <v>0.09706730378724263</v>
       </c>
       <c r="AU19">
         <v>1</v>
       </c>
       <c r="AV19" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
     </row>
     <row r="20" spans="1:48">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>128</v>
       </c>
       <c r="B20">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
         <v>256</v>
       </c>
       <c r="D20" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E20">
-        <v>596771</v>
+        <v>60055924</v>
       </c>
       <c r="F20">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G20" t="s">
-        <v>168</v>
+        <v>128</v>
       </c>
       <c r="H20" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="I20" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="J20">
         <v>1</v>
       </c>
       <c r="K20" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="L20">
-        <v>13.88493150684931</v>
+        <v>10.01369863013699</v>
       </c>
       <c r="M20" t="s">
-        <v>264</v>
+        <v>274</v>
       </c>
       <c r="N20">
-        <v>-0.04714682046984989</v>
+        <v>-0.03946400935227341</v>
       </c>
       <c r="O20">
-        <v>-0.0487858486740003</v>
+        <v>-0.04170725587089447</v>
       </c>
       <c r="P20">
-        <v>-0.04896253477920987</v>
+        <v>-0.04374958793004801</v>
       </c>
       <c r="Q20">
-        <v>-0.04896253477920987</v>
+        <v>-0.04562856661191542</v>
       </c>
       <c r="R20">
-        <v>-0.04896253477920987</v>
+        <v>-0.04736839890979524</v>
       </c>
       <c r="S20">
         <v>-0.04896253477920987</v>
@@ -7128,207 +7287,645 @@
         <v>-0.04896253477920987</v>
       </c>
       <c r="AD20">
-        <v>-0.0361370479186777</v>
+        <v>-0.04361157366410478</v>
       </c>
       <c r="AE20">
-        <v>-0.03593849478630882</v>
+        <v>-0.03756930381072473</v>
       </c>
       <c r="AF20">
-        <v>-0.0361370479186777</v>
+        <v>-0.03927017866165177</v>
       </c>
       <c r="AG20">
-        <v>-0.0361370479186777</v>
+        <v>-0.04083501116334636</v>
       </c>
       <c r="AH20">
-        <v>-0.0361370479186777</v>
+        <v>-0.04228396114531983</v>
       </c>
       <c r="AI20">
-        <v>-0.0361370479186777</v>
+        <v>-0.04361157366410478</v>
       </c>
       <c r="AJ20">
-        <v>-0.0361370479186777</v>
+        <v>-0.04361157366410478</v>
       </c>
       <c r="AK20">
-        <v>-0.0361370479186777</v>
+        <v>-0.04361157366410478</v>
       </c>
       <c r="AL20">
-        <v>-0.0361370479186777</v>
+        <v>-0.04361157366410478</v>
       </c>
       <c r="AM20">
-        <v>-0.0361370479186777</v>
+        <v>-0.04361157366410478</v>
       </c>
       <c r="AN20">
-        <v>-0.0361370479186777</v>
+        <v>-0.04361157366410478</v>
       </c>
       <c r="AO20">
-        <v>-0.0361370479186777</v>
+        <v>-0.04361157366410478</v>
       </c>
       <c r="AP20">
-        <v>-0.0361370479186777</v>
+        <v>-0.04361157366410478</v>
       </c>
       <c r="AQ20">
-        <v>-0.0361370479186777</v>
+        <v>-0.04361157366410478</v>
       </c>
       <c r="AR20">
-        <v>-0.0361370479186777</v>
+        <v>-0.04361157366410478</v>
       </c>
       <c r="AS20">
-        <v>-0.0361370479186777</v>
+        <v>-0.04361157366410478</v>
       </c>
       <c r="AT20">
-        <v>0.5442759034755772</v>
+        <v>0.7395372742482074</v>
       </c>
       <c r="AU20">
         <v>1</v>
       </c>
       <c r="AV20" t="s">
-        <v>272</v>
+        <v>277</v>
       </c>
     </row>
     <row r="21" spans="1:48">
       <c r="A21" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="B21">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="C21" t="s">
         <v>257</v>
       </c>
       <c r="D21" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="E21">
-        <v>60168413</v>
+        <v>60144910</v>
       </c>
       <c r="F21">
-        <v>11</v>
+        <v>37</v>
       </c>
       <c r="G21" t="s">
-        <v>114</v>
+        <v>128</v>
       </c>
       <c r="H21" t="s">
-        <v>263</v>
+        <v>265</v>
       </c>
       <c r="I21" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="J21">
         <v>1</v>
       </c>
       <c r="K21" t="s">
-        <v>268</v>
+        <v>272</v>
       </c>
       <c r="L21">
-        <v>6.397260273972603</v>
+        <v>7.317808219178082</v>
       </c>
       <c r="M21" t="s">
         <v>270</v>
       </c>
       <c r="N21">
+        <v>-0.006647356104413221</v>
+      </c>
+      <c r="O21">
+        <v>-0.008158156386945684</v>
+      </c>
+      <c r="P21">
+        <v>-0.009493379801801163</v>
+      </c>
+      <c r="Q21">
+        <v>-0.01069239212509018</v>
+      </c>
+      <c r="R21">
+        <v>-0.01178042952012766</v>
+      </c>
+      <c r="S21">
+        <v>-0.01277892143247003</v>
+      </c>
+      <c r="T21">
+        <v>-0.01369684080868297</v>
+      </c>
+      <c r="U21">
+        <v>-0.01454829609654285</v>
+      </c>
+      <c r="V21">
+        <v>-0.01509139912581338</v>
+      </c>
+      <c r="W21">
+        <v>-0.01509139912581338</v>
+      </c>
+      <c r="X21">
+        <v>-0.01509139912581338</v>
+      </c>
+      <c r="Y21">
+        <v>-0.01509139912581338</v>
+      </c>
+      <c r="Z21">
+        <v>-0.01509139912581338</v>
+      </c>
+      <c r="AA21">
+        <v>-0.01509139912581338</v>
+      </c>
+      <c r="AB21">
+        <v>-0.01509139912581338</v>
+      </c>
+      <c r="AC21">
+        <v>-0.01509139912581338</v>
+      </c>
+      <c r="AD21">
+        <v>-0.02</v>
+      </c>
+      <c r="AE21">
+        <v>-0.02</v>
+      </c>
+      <c r="AF21">
+        <v>-0.02</v>
+      </c>
+      <c r="AG21">
+        <v>-0.02</v>
+      </c>
+      <c r="AH21">
+        <v>-0.02</v>
+      </c>
+      <c r="AI21">
+        <v>-0.02</v>
+      </c>
+      <c r="AJ21">
+        <v>-0.02</v>
+      </c>
+      <c r="AK21">
+        <v>-0.02</v>
+      </c>
+      <c r="AL21">
+        <v>-0.02</v>
+      </c>
+      <c r="AM21">
+        <v>-0.02</v>
+      </c>
+      <c r="AN21">
+        <v>-0.02</v>
+      </c>
+      <c r="AO21">
+        <v>-0.02</v>
+      </c>
+      <c r="AP21">
+        <v>-0.02</v>
+      </c>
+      <c r="AQ21">
+        <v>-0.02</v>
+      </c>
+      <c r="AR21">
+        <v>-0.02</v>
+      </c>
+      <c r="AS21">
+        <v>-0.02</v>
+      </c>
+      <c r="AT21">
+        <v>0.2475980482608367</v>
+      </c>
+      <c r="AU21">
+        <v>1</v>
+      </c>
+      <c r="AV21" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="22" spans="1:48">
+      <c r="A22" t="s">
+        <v>122</v>
+      </c>
+      <c r="B22">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>258</v>
+      </c>
+      <c r="D22" t="s">
+        <v>261</v>
+      </c>
+      <c r="E22">
+        <v>496678</v>
+      </c>
+      <c r="F22">
+        <v>9</v>
+      </c>
+      <c r="G22" t="s">
+        <v>122</v>
+      </c>
+      <c r="H22" t="s">
+        <v>266</v>
+      </c>
+      <c r="I22" t="s">
+        <v>261</v>
+      </c>
+      <c r="J22">
+        <v>1</v>
+      </c>
+      <c r="K22" t="s">
+        <v>273</v>
+      </c>
+      <c r="L22">
+        <v>14.62191780821918</v>
+      </c>
+      <c r="M22" t="s">
+        <v>268</v>
+      </c>
+      <c r="N22">
+        <v>-0.04836247008897316</v>
+      </c>
+      <c r="O22">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="P22">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="Q22">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="R22">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="S22">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="T22">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="U22">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="V22">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="W22">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="X22">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="Y22">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="Z22">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="AA22">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="AB22">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="AC22">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="AD22">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AE22">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AF22">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AG22">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AH22">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AI22">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AJ22">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AK22">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AL22">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AM22">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AN22">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AO22">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AP22">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AQ22">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AR22">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AS22">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AT22">
+        <v>0.4573823720901941</v>
+      </c>
+      <c r="AU22">
+        <v>1</v>
+      </c>
+      <c r="AV22" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="23" spans="1:48">
+      <c r="A23" t="s">
+        <v>168</v>
+      </c>
+      <c r="B23">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>259</v>
+      </c>
+      <c r="D23" t="s">
+        <v>261</v>
+      </c>
+      <c r="E23">
+        <v>596771</v>
+      </c>
+      <c r="F23">
+        <v>11</v>
+      </c>
+      <c r="G23" t="s">
+        <v>168</v>
+      </c>
+      <c r="H23" t="s">
+        <v>266</v>
+      </c>
+      <c r="I23" t="s">
+        <v>261</v>
+      </c>
+      <c r="J23">
+        <v>1</v>
+      </c>
+      <c r="K23" t="s">
+        <v>273</v>
+      </c>
+      <c r="L23">
+        <v>13.88493150684931</v>
+      </c>
+      <c r="M23" t="s">
+        <v>268</v>
+      </c>
+      <c r="N23">
+        <v>-0.04714682046984989</v>
+      </c>
+      <c r="O23">
+        <v>-0.0487858486740003</v>
+      </c>
+      <c r="P23">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="Q23">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="R23">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="S23">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="T23">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="U23">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="V23">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="W23">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="X23">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="Y23">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="Z23">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="AA23">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="AB23">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="AC23">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="AD23">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AE23">
+        <v>-0.03593849478630882</v>
+      </c>
+      <c r="AF23">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AG23">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AH23">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AI23">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AJ23">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AK23">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AL23">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AM23">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AN23">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AO23">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AP23">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AQ23">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AR23">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AS23">
+        <v>-0.0361370479186777</v>
+      </c>
+      <c r="AT23">
+        <v>0.5442759034755772</v>
+      </c>
+      <c r="AU23">
+        <v>1</v>
+      </c>
+      <c r="AV23" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="24" spans="1:48">
+      <c r="A24" t="s">
+        <v>114</v>
+      </c>
+      <c r="B24">
+        <v>19</v>
+      </c>
+      <c r="C24" t="s">
+        <v>260</v>
+      </c>
+      <c r="D24" t="s">
+        <v>261</v>
+      </c>
+      <c r="E24">
+        <v>60168413</v>
+      </c>
+      <c r="F24">
+        <v>11</v>
+      </c>
+      <c r="G24" t="s">
+        <v>114</v>
+      </c>
+      <c r="H24" t="s">
+        <v>267</v>
+      </c>
+      <c r="I24" t="s">
+        <v>261</v>
+      </c>
+      <c r="J24">
+        <v>1</v>
+      </c>
+      <c r="K24" t="s">
+        <v>273</v>
+      </c>
+      <c r="L24">
+        <v>6.397260273972603</v>
+      </c>
+      <c r="M24" t="s">
+        <v>274</v>
+      </c>
+      <c r="N24">
         <v>-0.02893151889286374</v>
       </c>
-      <c r="O21">
+      <c r="O24">
         <v>-0.03235417441917252</v>
       </c>
-      <c r="P21">
+      <c r="P24">
         <v>-0.03533355000116906</v>
       </c>
-      <c r="Q21">
+      <c r="Q24">
         <v>-0.03797741310063497</v>
       </c>
-      <c r="R21">
+      <c r="R24">
         <v>-0.04035373853564519</v>
       </c>
-      <c r="S21">
+      <c r="S24">
         <v>-0.04251737891437576</v>
       </c>
-      <c r="T21">
+      <c r="T24">
         <v>-0.04449334803022762</v>
       </c>
-      <c r="U21">
+      <c r="U24">
         <v>-0.0463160137963143</v>
       </c>
-      <c r="V21">
+      <c r="V24">
         <v>-0.04800746080439115</v>
       </c>
-      <c r="W21">
-        <v>-0.04896253477920987</v>
-      </c>
-      <c r="X21">
-        <v>-0.04896253477920987</v>
-      </c>
-      <c r="Y21">
-        <v>-0.04896253477920987</v>
-      </c>
-      <c r="Z21">
-        <v>-0.04896253477920987</v>
-      </c>
-      <c r="AA21">
-        <v>-0.04896253477920987</v>
-      </c>
-      <c r="AB21">
-        <v>-0.04896253477920987</v>
-      </c>
-      <c r="AC21">
-        <v>-0.04896253477920987</v>
-      </c>
-      <c r="AD21">
+      <c r="W24">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="X24">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="Y24">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="Z24">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="AA24">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="AB24">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="AC24">
+        <v>-0.04896253477920987</v>
+      </c>
+      <c r="AD24">
         <v>-0.04361157366410478</v>
       </c>
-      <c r="AE21">
+      <c r="AE24">
         <v>-0.02977996272458456</v>
       </c>
-      <c r="AF21">
+      <c r="AF24">
         <v>-0.03226121692424899</v>
       </c>
-      <c r="AG21">
+      <c r="AG24">
         <v>-0.03446305292590255</v>
       </c>
-      <c r="AH21">
+      <c r="AH24">
         <v>-0.03644208084739651</v>
       </c>
-      <c r="AI21">
+      <c r="AI24">
         <v>-0.03824398249710099</v>
       </c>
-      <c r="AJ21">
+      <c r="AJ24">
         <v>-0.03988958961583459</v>
       </c>
-      <c r="AK21">
+      <c r="AK24">
         <v>-0.04140752415017635</v>
       </c>
-      <c r="AL21">
+      <c r="AL24">
         <v>-0.04281617837210835</v>
       </c>
-      <c r="AM21">
+      <c r="AM24">
         <v>-0.04361157366410478</v>
       </c>
-      <c r="AN21">
+      <c r="AN24">
         <v>-0.04361157366410478</v>
       </c>
-      <c r="AO21">
+      <c r="AO24">
         <v>-0.04361157366410478</v>
       </c>
-      <c r="AP21">
+      <c r="AP24">
         <v>-0.04361157366410478</v>
       </c>
-      <c r="AQ21">
+      <c r="AQ24">
         <v>-0.04361157366410478</v>
       </c>
-      <c r="AR21">
+      <c r="AR24">
         <v>-0.04361157366410478</v>
       </c>
-      <c r="AS21">
+      <c r="AS24">
         <v>-0.04361157366410478</v>
       </c>
-      <c r="AT21">
+      <c r="AT24">
         <v>0.3277283878667971</v>
       </c>
-      <c r="AU21">
-        <v>1</v>
-      </c>
-      <c r="AV21" t="s">
-        <v>273</v>
+      <c r="AU24">
+        <v>1</v>
+      </c>
+      <c r="AV24" t="s">
+        <v>277</v>
       </c>
     </row>
   </sheetData>
@@ -7352,34 +7949,34 @@
         <v>196</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>274</v>
+        <v>279</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>275</v>
+        <v>280</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>276</v>
+        <v>281</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>277</v>
+        <v>282</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>278</v>
+        <v>283</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>279</v>
+        <v>284</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>280</v>
+        <v>285</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>281</v>
+        <v>286</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>282</v>
+        <v>287</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>283</v>
+        <v>288</v>
       </c>
     </row>
     <row r="2" spans="1:12">
@@ -7390,34 +7987,34 @@
         <v>121</v>
       </c>
       <c r="C2">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D2">
-        <v>9.626418786692758</v>
+        <v>8.263819500402901</v>
       </c>
       <c r="E2">
-        <v>201</v>
+        <v>374</v>
       </c>
       <c r="F2">
-        <v>3.045636329696092</v>
+        <v>6.576248574594051</v>
       </c>
       <c r="G2">
-        <v>-7.220844176944153</v>
+        <v>-3.690231932046194</v>
       </c>
       <c r="H2">
-        <v>6.479401864686803</v>
+        <v>10.01001410958476</v>
       </c>
       <c r="I2">
-        <v>-0.01492625073723687</v>
+        <v>-0.01727971359017978</v>
       </c>
       <c r="J2">
-        <v>0.03726326573296496</v>
+        <v>0.009965256793790588</v>
       </c>
       <c r="K2">
-        <v>-0.03122913314022622</v>
+        <v>-0.02606706528941771</v>
       </c>
       <c r="L2">
-        <v>0.06849239887319117</v>
+        <v>0.0360323220832083</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -7425,34 +8022,34 @@
         <v>121</v>
       </c>
       <c r="C3">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="D3">
-        <v>9.626418786692758</v>
+        <v>8.263819500402901</v>
       </c>
       <c r="E3">
-        <v>201</v>
+        <v>374</v>
       </c>
       <c r="F3">
-        <v>3.045636329696092</v>
+        <v>6.576248574594051</v>
       </c>
       <c r="G3">
-        <v>-7.220844176944153</v>
+        <v>-3.690231932046194</v>
       </c>
       <c r="H3">
-        <v>6.479401864686803</v>
+        <v>10.01001410958476</v>
       </c>
       <c r="I3">
-        <v>-0.01492625073723687</v>
+        <v>-0.01727971359017978</v>
       </c>
       <c r="J3">
-        <v>0.03726326573296496</v>
+        <v>0.009965256793790588</v>
       </c>
       <c r="K3">
-        <v>-0.03122913314022622</v>
+        <v>-0.02606706528941771</v>
       </c>
       <c r="L3">
-        <v>0.006849239887319117</v>
+        <v>0.00360323220832083</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -7754,7 +8351,7 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O12"/>
+  <dimension ref="A1:O13"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -7783,28 +8380,28 @@
         <v>199</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>284</v>
+        <v>289</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>285</v>
+        <v>290</v>
       </c>
       <c r="J1" s="1" t="s">
+        <v>291</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>292</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>286</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>287</v>
       </c>
-      <c r="L1" s="1" t="s">
-        <v>281</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>282</v>
-      </c>
       <c r="N1" s="1" t="s">
-        <v>288</v>
+        <v>293</v>
       </c>
       <c r="O1" s="1" t="s">
-        <v>289</v>
+        <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -7815,25 +8412,25 @@
         <v>121</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>272</v>
+        <v>278</v>
       </c>
       <c r="E2" t="s">
-        <v>258</v>
+        <v>270</v>
       </c>
       <c r="F2" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="G2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H2">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I2">
-        <v>61</v>
+        <v>173</v>
       </c>
       <c r="J2">
         <v>0.5</v>
@@ -7842,16 +8439,16 @@
         <v>10.5</v>
       </c>
       <c r="L2">
-        <v>0.030984668908323</v>
+        <v>-0.02</v>
       </c>
       <c r="M2">
-        <v>-0.04057867427553811</v>
+        <v>-0.02</v>
       </c>
       <c r="N2">
-        <v>-1.833261793707401</v>
+        <v>3.530612244897959</v>
       </c>
       <c r="O2">
-        <v>2.579991776750135</v>
+        <v>3.530612244897959</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -7865,22 +8462,22 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="E3" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F3" t="s">
-        <v>264</v>
+        <v>273</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
       <c r="H3">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="I3">
-        <v>66</v>
+        <v>61</v>
       </c>
       <c r="J3">
         <v>0.5</v>
@@ -7889,16 +8486,16 @@
         <v>10.5</v>
       </c>
       <c r="L3">
-        <v>0.05370458222796941</v>
+        <v>0.030984668908323</v>
       </c>
       <c r="M3">
-        <v>-0.02671558400461935</v>
+        <v>-0.04057867427553811</v>
       </c>
       <c r="N3">
-        <v>-3.363848356387926</v>
+        <v>-1.833261793707401</v>
       </c>
       <c r="O3">
-        <v>1.811627223581525</v>
+        <v>2.579991776750135</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -7912,10 +8509,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>273</v>
+        <v>276</v>
       </c>
       <c r="E4" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="F4" t="s">
         <v>268</v>
@@ -7927,7 +8524,7 @@
         <v>3</v>
       </c>
       <c r="I4">
-        <v>42</v>
+        <v>66</v>
       </c>
       <c r="J4">
         <v>0.5</v>
@@ -7936,16 +8533,16 @@
         <v>10.5</v>
       </c>
       <c r="L4">
-        <v>0.030984668908323</v>
+        <v>0.05370458222796941</v>
       </c>
       <c r="M4">
-        <v>-0.04057867427553811</v>
+        <v>-0.02671558400461935</v>
       </c>
       <c r="N4">
-        <v>-1.262245825175587</v>
+        <v>-3.363848356387926</v>
       </c>
       <c r="O4">
-        <v>1.776387780713208</v>
+        <v>1.811627223581525</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -7959,22 +8556,22 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="E5" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="F5" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="G5">
         <v>1</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I5">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="J5">
         <v>0.5</v>
@@ -7983,16 +8580,16 @@
         <v>10.5</v>
       </c>
       <c r="L5">
-        <v>0.02492292829285174</v>
+        <v>0.030984668908323</v>
       </c>
       <c r="M5">
-        <v>-0.01089519808621839</v>
+        <v>-0.04057867427553811</v>
       </c>
       <c r="N5">
-        <v>-0.3161194455340514</v>
+        <v>-1.262245825175587</v>
       </c>
       <c r="O5">
-        <v>0.1431977428951814</v>
+        <v>1.776387780713208</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -8006,13 +8603,13 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>271</v>
+        <v>275</v>
       </c>
       <c r="E6" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="F6" t="s">
-        <v>265</v>
+        <v>272</v>
       </c>
       <c r="G6">
         <v>1</v>
@@ -8021,7 +8618,7 @@
         <v>1</v>
       </c>
       <c r="I6">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="J6">
         <v>0.5</v>
@@ -8030,36 +8627,36 @@
         <v>10.5</v>
       </c>
       <c r="L6">
-        <v>0.02400310468506598</v>
+        <v>0.02492292829285174</v>
       </c>
       <c r="M6">
-        <v>-0.008774812662701914</v>
+        <v>-0.01089519808621839</v>
       </c>
       <c r="N6">
-        <v>-0.4453687561391871</v>
+        <v>-0.3161194455340514</v>
       </c>
       <c r="O6">
-        <v>0.1681973407467538</v>
+        <v>0.1431977428951814</v>
       </c>
     </row>
     <row r="7" spans="1:15">
       <c r="A7" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="B7" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C7">
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>272</v>
+        <v>275</v>
       </c>
       <c r="E7" t="s">
-        <v>258</v>
+        <v>271</v>
       </c>
       <c r="F7" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -8068,7 +8665,7 @@
         <v>1</v>
       </c>
       <c r="I7">
-        <v>2</v>
+        <v>19</v>
       </c>
       <c r="J7">
         <v>0.5</v>
@@ -8077,16 +8674,16 @@
         <v>10.5</v>
       </c>
       <c r="L7">
-        <v>0.030984668908323</v>
+        <v>0.02400310468506598</v>
       </c>
       <c r="M7">
-        <v>-0.04057867427553811</v>
+        <v>-0.008774812662701914</v>
       </c>
       <c r="N7">
-        <v>-0.06010694405598035</v>
+        <v>-0.4453687561391871</v>
       </c>
       <c r="O7">
-        <v>0.08458989431967656</v>
+        <v>0.1681973407467538</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -8100,14 +8697,14 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
+        <v>276</v>
+      </c>
+      <c r="E8" t="s">
+        <v>261</v>
+      </c>
+      <c r="F8" t="s">
         <v>273</v>
       </c>
-      <c r="E8" t="s">
-        <v>258</v>
-      </c>
-      <c r="F8" t="s">
-        <v>268</v>
-      </c>
       <c r="G8">
         <v>1</v>
       </c>
@@ -8115,7 +8712,7 @@
         <v>1</v>
       </c>
       <c r="I8">
-        <v>18</v>
+        <v>2</v>
       </c>
       <c r="J8">
         <v>0.5</v>
@@ -8130,10 +8727,10 @@
         <v>-0.04057867427553811</v>
       </c>
       <c r="N8">
-        <v>-0.5409624965038232</v>
+        <v>-0.06010694405598035</v>
       </c>
       <c r="O8">
-        <v>0.7613090488770891</v>
+        <v>0.08458989431967656</v>
       </c>
     </row>
     <row r="9" spans="1:15">
@@ -8147,13 +8744,13 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>271</v>
+        <v>277</v>
       </c>
       <c r="E9" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="F9" t="s">
-        <v>267</v>
+        <v>273</v>
       </c>
       <c r="G9">
         <v>1</v>
@@ -8162,7 +8759,7 @@
         <v>1</v>
       </c>
       <c r="I9">
-        <v>37</v>
+        <v>18</v>
       </c>
       <c r="J9">
         <v>0.5</v>
@@ -8171,37 +8768,37 @@
         <v>10.5</v>
       </c>
       <c r="L9">
-        <v>0.02492292829285174</v>
+        <v>0.030984668908323</v>
       </c>
       <c r="M9">
-        <v>-0.01089519808621839</v>
+        <v>-0.04057867427553811</v>
       </c>
       <c r="N9">
-        <v>-0.8997245757507616</v>
+        <v>-0.5409624965038232</v>
       </c>
       <c r="O9">
-        <v>0.4075628067016702</v>
+        <v>0.7613090488770891</v>
       </c>
     </row>
     <row r="10" spans="1:15">
       <c r="A10" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="B10" t="s">
-        <v>122</v>
+        <v>128</v>
       </c>
       <c r="C10">
         <v>1</v>
       </c>
       <c r="D10" t="s">
+        <v>275</v>
+      </c>
+      <c r="E10" t="s">
+        <v>261</v>
+      </c>
+      <c r="F10" t="s">
         <v>272</v>
       </c>
-      <c r="E10" t="s">
-        <v>258</v>
-      </c>
-      <c r="F10" t="s">
-        <v>268</v>
-      </c>
       <c r="G10">
         <v>1</v>
       </c>
@@ -8209,7 +8806,7 @@
         <v>1</v>
       </c>
       <c r="I10">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="J10">
         <v>0.5</v>
@@ -8218,36 +8815,36 @@
         <v>10.5</v>
       </c>
       <c r="L10">
-        <v>0.030984668908323</v>
+        <v>0.02492292829285174</v>
       </c>
       <c r="M10">
-        <v>-0.04057867427553811</v>
+        <v>-0.01089519808621839</v>
       </c>
       <c r="N10">
-        <v>-0.2704812482519116</v>
+        <v>-0.8997245757507616</v>
       </c>
       <c r="O10">
-        <v>0.3806545244385445</v>
+        <v>0.4075628067016702</v>
       </c>
     </row>
     <row r="11" spans="1:15">
       <c r="A11" t="s">
-        <v>168</v>
+        <v>122</v>
       </c>
       <c r="B11" t="s">
-        <v>168</v>
+        <v>122</v>
       </c>
       <c r="C11">
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>272</v>
+        <v>276</v>
       </c>
       <c r="E11" t="s">
-        <v>258</v>
+        <v>261</v>
       </c>
       <c r="F11" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="G11">
         <v>1</v>
@@ -8256,7 +8853,7 @@
         <v>1</v>
       </c>
       <c r="I11">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="J11">
         <v>0.5</v>
@@ -8271,30 +8868,30 @@
         <v>-0.04057867427553811</v>
       </c>
       <c r="N11">
-        <v>-0.3305881923078919</v>
+        <v>-0.2704812482519116</v>
       </c>
       <c r="O11">
-        <v>0.4652444187582211</v>
+        <v>0.3806545244385445</v>
       </c>
     </row>
     <row r="12" spans="1:15">
       <c r="A12" t="s">
-        <v>114</v>
+        <v>168</v>
       </c>
       <c r="B12" t="s">
-        <v>114</v>
+        <v>168</v>
       </c>
       <c r="C12">
         <v>1</v>
       </c>
       <c r="D12" t="s">
+        <v>276</v>
+      </c>
+      <c r="E12" t="s">
+        <v>261</v>
+      </c>
+      <c r="F12" t="s">
         <v>273</v>
-      </c>
-      <c r="E12" t="s">
-        <v>258</v>
-      </c>
-      <c r="F12" t="s">
-        <v>268</v>
       </c>
       <c r="G12">
         <v>1</v>
@@ -8321,6 +8918,53 @@
         <v>-0.3305881923078919</v>
       </c>
       <c r="O12">
+        <v>0.4652444187582211</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
+      <c r="A13" t="s">
+        <v>114</v>
+      </c>
+      <c r="B13" t="s">
+        <v>114</v>
+      </c>
+      <c r="C13">
+        <v>1</v>
+      </c>
+      <c r="D13" t="s">
+        <v>277</v>
+      </c>
+      <c r="E13" t="s">
+        <v>261</v>
+      </c>
+      <c r="F13" t="s">
+        <v>273</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+      <c r="I13">
+        <v>11</v>
+      </c>
+      <c r="J13">
+        <v>0.5</v>
+      </c>
+      <c r="K13">
+        <v>10.5</v>
+      </c>
+      <c r="L13">
+        <v>0.030984668908323</v>
+      </c>
+      <c r="M13">
+        <v>-0.04057867427553811</v>
+      </c>
+      <c r="N13">
+        <v>-0.3305881923078919</v>
+      </c>
+      <c r="O13">
         <v>0.4652444187582211</v>
       </c>
     </row>

</xml_diff>

<commit_message>
test changes (maybe revert this one)
</commit_message>
<xml_diff>
--- a/Code/Limpio/Excels/preprocessed/preprocessed_mm_modelo MM - TALCA 28.12_v4.xlsx
+++ b/Code/Limpio/Excels/preprocessed/preprocessed_mm_modelo MM - TALCA 28.12_v4.xlsx
@@ -734,6 +734,15 @@
     <t>DN</t>
   </si>
   <si>
+    <t>16/02/2022</t>
+  </si>
+  <si>
+    <t>20/01/2021</t>
+  </si>
+  <si>
+    <t>03/11/2020</t>
+  </si>
+  <si>
     <t>22/12/2020</t>
   </si>
   <si>
@@ -776,15 +785,6 @@
     <t>12/05/2022</t>
   </si>
   <si>
-    <t>16/02/2022</t>
-  </si>
-  <si>
-    <t>20/01/2021</t>
-  </si>
-  <si>
-    <t>03/11/2020</t>
-  </si>
-  <si>
     <t>13/11/2009</t>
   </si>
   <si>
@@ -803,6 +803,9 @@
     <t>07/11/2016</t>
   </si>
   <si>
+    <t>R800</t>
+  </si>
+  <si>
     <t>B</t>
   </si>
   <si>
@@ -812,7 +815,7 @@
     <t>R315</t>
   </si>
   <si>
-    <t>R800</t>
+    <t>ULTRA</t>
   </si>
   <si>
     <t>B-25</t>
@@ -830,9 +833,6 @@
     <t>C-25</t>
   </si>
   <si>
-    <t>ULTRA</t>
-  </si>
-  <si>
     <t>C</t>
   </si>
   <si>
@@ -845,6 +845,9 @@
     <t>C-19</t>
   </si>
   <si>
+    <t>38</t>
+  </si>
+  <si>
     <t>25</t>
   </si>
   <si>
@@ -852,9 +855,6 @@
   </si>
   <si>
     <t>19</t>
-  </si>
-  <si>
-    <t>38</t>
   </si>
   <si>
     <t>N_medidores</t>
@@ -4575,7 +4575,7 @@
         <v>121</v>
       </c>
       <c r="B2">
-        <v>25</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
         <v>238</v>
@@ -4584,10 +4584,10 @@
         <v>261</v>
       </c>
       <c r="E2">
-        <v>60274432</v>
+        <v>345317</v>
       </c>
       <c r="F2">
-        <v>13</v>
+        <v>124</v>
       </c>
       <c r="G2" t="s">
         <v>121</v>
@@ -4596,67 +4596,67 @@
         <v>265</v>
       </c>
       <c r="I2" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K2" t="s">
-        <v>272</v>
+        <v>265</v>
       </c>
       <c r="L2">
-        <v>2.271232876712329</v>
+        <v>0.5</v>
       </c>
       <c r="M2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="N2">
-        <v>0.007117292039837499</v>
+        <v>-0.02</v>
       </c>
       <c r="O2">
-        <v>0.002815133124474241</v>
+        <v>-0.02</v>
       </c>
       <c r="P2">
-        <v>-0.0003206461506646691</v>
+        <v>-0.02</v>
       </c>
       <c r="Q2">
-        <v>-0.002794074509479778</v>
+        <v>-0.02</v>
       </c>
       <c r="R2">
-        <v>-0.00483674384727116</v>
+        <v>-0.02</v>
       </c>
       <c r="S2">
-        <v>-0.006581100382378358</v>
+        <v>-0.02</v>
       </c>
       <c r="T2">
-        <v>-0.008096011499679756</v>
+        <v>-0.02</v>
       </c>
       <c r="U2">
-        <v>-0.0094379181711442</v>
+        <v>-0.02</v>
       </c>
       <c r="V2">
-        <v>-0.01064231585213564</v>
+        <v>-0.02</v>
       </c>
       <c r="W2">
-        <v>-0.01173764328089111</v>
+        <v>-0.02</v>
       </c>
       <c r="X2">
-        <v>-0.01273699790796427</v>
+        <v>-0.02</v>
       </c>
       <c r="Y2">
-        <v>-0.01365806911018531</v>
+        <v>-0.02</v>
       </c>
       <c r="Z2">
-        <v>-0.0145122354503333</v>
+        <v>-0.02</v>
       </c>
       <c r="AA2">
-        <v>-0.01509139912581338</v>
+        <v>-0.02</v>
       </c>
       <c r="AB2">
-        <v>-0.01509139912581338</v>
+        <v>-0.02</v>
       </c>
       <c r="AC2">
-        <v>-0.01509139912581338</v>
+        <v>-0.02</v>
       </c>
       <c r="AD2">
         <v>-0.02</v>
@@ -4707,10 +4707,10 @@
         <v>-0.02</v>
       </c>
       <c r="AT2">
-        <v>-0.09187092431953553</v>
+        <v>2.530612244897959</v>
       </c>
       <c r="AU2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV2" t="s">
         <v>275</v>
@@ -4721,7 +4721,7 @@
         <v>121</v>
       </c>
       <c r="B3">
-        <v>13</v>
+        <v>38</v>
       </c>
       <c r="C3" t="s">
         <v>239</v>
@@ -4730,136 +4730,136 @@
         <v>261</v>
       </c>
       <c r="E3">
-        <v>1252181</v>
+        <v>941780</v>
       </c>
       <c r="F3">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="G3" t="s">
         <v>121</v>
       </c>
       <c r="H3" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="I3" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="J3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K3" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="L3">
-        <v>13.41369863013699</v>
+        <v>1.526027397260274</v>
       </c>
       <c r="M3" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="N3">
-        <v>-0.04633522557134629</v>
+        <v>-0.02</v>
       </c>
       <c r="O3">
-        <v>-0.04802980666161467</v>
+        <v>-0.02</v>
       </c>
       <c r="P3">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="Q3">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="R3">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="S3">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="T3">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="U3">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="V3">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="W3">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="X3">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="Y3">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="Z3">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="AA3">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="AB3">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="AC3">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="AD3">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AE3">
-        <v>-0.03508888349636861</v>
+        <v>-0.02</v>
       </c>
       <c r="AF3">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AG3">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AH3">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AI3">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AJ3">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AK3">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AL3">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AM3">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AN3">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AO3">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AP3">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AQ3">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AR3">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AS3">
-        <v>-0.0361370479186777</v>
+        <v>-0.02</v>
       </c>
       <c r="AT3">
-        <v>0.5344514078232218</v>
+        <v>0.3673469387755102</v>
       </c>
       <c r="AU3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV3" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="4" spans="1:48">
@@ -4867,7 +4867,7 @@
         <v>121</v>
       </c>
       <c r="B4">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="C4" t="s">
         <v>240</v>
@@ -4876,136 +4876,136 @@
         <v>261</v>
       </c>
       <c r="E4">
-        <v>60209133</v>
+        <v>941731</v>
       </c>
       <c r="F4">
-        <v>13</v>
+        <v>31</v>
       </c>
       <c r="G4" t="s">
         <v>121</v>
       </c>
       <c r="H4" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="I4" t="s">
-        <v>261</v>
+        <v>265</v>
       </c>
       <c r="J4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K4" t="s">
-        <v>273</v>
+        <v>265</v>
       </c>
       <c r="L4">
-        <v>4.794520547945205</v>
+        <v>1.73972602739726</v>
       </c>
       <c r="M4" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
       <c r="N4">
-        <v>-0.0221525938800527</v>
+        <v>-0.02</v>
       </c>
       <c r="O4">
-        <v>-0.0266165839818563</v>
+        <v>-0.02</v>
       </c>
       <c r="P4">
-        <v>-0.03035712948128109</v>
+        <v>-0.02</v>
       </c>
       <c r="Q4">
-        <v>-0.03358333952552957</v>
+        <v>-0.02</v>
       </c>
       <c r="R4">
-        <v>-0.03641971193549965</v>
+        <v>-0.02</v>
       </c>
       <c r="S4">
-        <v>-0.03895695505997775</v>
+        <v>-0.02</v>
       </c>
       <c r="T4">
-        <v>-0.04124084779450402</v>
+        <v>-0.02</v>
       </c>
       <c r="U4">
-        <v>-0.04332234901306013</v>
+        <v>-0.02</v>
       </c>
       <c r="V4">
-        <v>-0.04523442751858323</v>
+        <v>-0.02</v>
       </c>
       <c r="W4">
-        <v>-0.04700726570344111</v>
+        <v>-0.02</v>
       </c>
       <c r="X4">
-        <v>-0.04865136943504261</v>
+        <v>-0.02</v>
       </c>
       <c r="Y4">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="Z4">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="AA4">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="AB4">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="AC4">
-        <v>-0.04896253477920987</v>
+        <v>-0.02</v>
       </c>
       <c r="AD4">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AE4">
-        <v>-0.02500163922130701</v>
+        <v>-0.02</v>
       </c>
       <c r="AF4">
-        <v>-0.02811680344751848</v>
+        <v>-0.02</v>
       </c>
       <c r="AG4">
-        <v>-0.03080362389058822</v>
+        <v>-0.02</v>
       </c>
       <c r="AH4">
-        <v>-0.0331657835983396</v>
+        <v>-0.02</v>
       </c>
       <c r="AI4">
-        <v>-0.03527882540354973</v>
+        <v>-0.02</v>
       </c>
       <c r="AJ4">
-        <v>-0.0371808744346856</v>
+        <v>-0.02</v>
       </c>
       <c r="AK4">
-        <v>-0.03891436975879235</v>
+        <v>-0.02</v>
       </c>
       <c r="AL4">
-        <v>-0.04050676812930528</v>
+        <v>-0.02</v>
       </c>
       <c r="AM4">
-        <v>-0.04198320574867932</v>
+        <v>-0.02</v>
       </c>
       <c r="AN4">
-        <v>-0.0433524320098365</v>
+        <v>-0.02</v>
       </c>
       <c r="AO4">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AP4">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AQ4">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AR4">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AS4">
-        <v>-0.04361157366410478</v>
+        <v>-0.02</v>
       </c>
       <c r="AT4">
-        <v>0.2945078328564485</v>
+        <v>0.6326530612244898</v>
       </c>
       <c r="AU4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="AV4" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
     </row>
     <row r="5" spans="1:48">
@@ -5013,19 +5013,19 @@
         <v>121</v>
       </c>
       <c r="B5">
-        <v>13</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>241</v>
       </c>
       <c r="D5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E5">
-        <v>413560</v>
+        <v>60274432</v>
       </c>
       <c r="F5">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
         <v>121</v>
@@ -5034,118 +5034,118 @@
         <v>266</v>
       </c>
       <c r="I5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J5">
         <v>1</v>
       </c>
       <c r="K5" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="L5">
-        <v>15</v>
+        <v>1.605479452054795</v>
       </c>
       <c r="M5" t="s">
-        <v>268</v>
+        <v>265</v>
       </c>
       <c r="N5">
-        <v>-0.04896253477920987</v>
+        <v>-0.05048929843475818</v>
       </c>
       <c r="O5">
-        <v>-0.04896253477920987</v>
+        <v>-0.05618573589447737</v>
       </c>
       <c r="P5">
-        <v>-0.04896253477920987</v>
+        <v>-0.0600163193860011</v>
       </c>
       <c r="Q5">
-        <v>-0.04896253477920987</v>
+        <v>-0.06289430302781937</v>
       </c>
       <c r="R5">
-        <v>-0.04896253477920987</v>
+        <v>-0.06520480803827845</v>
       </c>
       <c r="S5">
-        <v>-0.04896253477920987</v>
+        <v>-0.0671351840228108</v>
       </c>
       <c r="T5">
-        <v>-0.04896253477920987</v>
+        <v>-0.06879725243281969</v>
       </c>
       <c r="U5">
-        <v>-0.04896253477920987</v>
+        <v>-0.07024957308784695</v>
       </c>
       <c r="V5">
-        <v>-0.04896253477920987</v>
+        <v>-0.07154214929082024</v>
       </c>
       <c r="W5">
-        <v>-0.04896253477920987</v>
+        <v>-0.07270666601008348</v>
       </c>
       <c r="X5">
-        <v>-0.04896253477920987</v>
+        <v>-0.07376900171283629</v>
       </c>
       <c r="Y5">
-        <v>-0.04896253477920987</v>
+        <v>-0.074740749890382</v>
       </c>
       <c r="Z5">
-        <v>-0.04896253477920987</v>
+        <v>-0.0756383214251533</v>
       </c>
       <c r="AA5">
-        <v>-0.04896253477920987</v>
+        <v>-0.07647224188758157</v>
       </c>
       <c r="AB5">
-        <v>-0.04896253477920987</v>
+        <v>-0.07677919490885256</v>
       </c>
       <c r="AC5">
-        <v>-0.04896253477920987</v>
+        <v>-0.07677919490885256</v>
       </c>
       <c r="AD5">
-        <v>-0.0361370479186777</v>
+        <v>-0.07677919490885256</v>
       </c>
       <c r="AE5">
-        <v>-0.0361370479186777</v>
+        <v>-0.05618573589447737</v>
       </c>
       <c r="AF5">
-        <v>-0.0361370479186777</v>
+        <v>-0.0600163193860011</v>
       </c>
       <c r="AG5">
-        <v>-0.0361370479186777</v>
+        <v>-0.06289430302781937</v>
       </c>
       <c r="AH5">
-        <v>-0.0361370479186777</v>
+        <v>-0.06520480803827845</v>
       </c>
       <c r="AI5">
-        <v>-0.0361370479186777</v>
+        <v>-0.0671351840228108</v>
       </c>
       <c r="AJ5">
-        <v>-0.0361370479186777</v>
+        <v>-0.06879725243281969</v>
       </c>
       <c r="AK5">
-        <v>-0.0361370479186777</v>
+        <v>-0.07024957308784695</v>
       </c>
       <c r="AL5">
-        <v>-0.0361370479186777</v>
+        <v>-0.07154214929082024</v>
       </c>
       <c r="AM5">
-        <v>-0.0361370479186777</v>
+        <v>-0.07270666601008348</v>
       </c>
       <c r="AN5">
-        <v>-0.0361370479186777</v>
+        <v>-0.07376900171283629</v>
       </c>
       <c r="AO5">
-        <v>-0.0361370479186777</v>
+        <v>-0.074740749890382</v>
       </c>
       <c r="AP5">
-        <v>-0.0361370479186777</v>
+        <v>-0.0756383214251533</v>
       </c>
       <c r="AQ5">
-        <v>-0.0361370479186777</v>
+        <v>-0.07647224188758157</v>
       </c>
       <c r="AR5">
-        <v>-0.0361370479186777</v>
+        <v>-0.07677919490885256</v>
       </c>
       <c r="AS5">
-        <v>-0.0361370479186777</v>
+        <v>-0.07677919490885256</v>
       </c>
       <c r="AT5">
-        <v>0.7722493051497641</v>
+        <v>0.6912622243960639</v>
       </c>
       <c r="AU5">
         <v>1</v>
@@ -5159,19 +5159,19 @@
         <v>121</v>
       </c>
       <c r="B6">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="C6" t="s">
         <v>242</v>
       </c>
       <c r="D6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E6">
-        <v>60177677</v>
+        <v>1252181</v>
       </c>
       <c r="F6">
-        <v>9</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
         <v>121</v>
@@ -5180,7 +5180,7 @@
         <v>267</v>
       </c>
       <c r="I6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J6">
         <v>1</v>
@@ -5189,109 +5189,109 @@
         <v>273</v>
       </c>
       <c r="L6">
-        <v>6.18082191780822</v>
+        <v>12.74794520547945</v>
       </c>
       <c r="M6" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="N6">
-        <v>-0.02812248986069876</v>
+        <v>-0.1031107561695989</v>
       </c>
       <c r="O6">
-        <v>-0.03165641782081328</v>
+        <v>-0.1048858824530204</v>
       </c>
       <c r="P6">
-        <v>-0.03471995400676191</v>
+        <v>-0.1065406804703833</v>
       </c>
       <c r="Q6">
-        <v>-0.03742985986465747</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="R6">
-        <v>-0.03985939239596478</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="S6">
-        <v>-0.04206692417585865</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="T6">
-        <v>-0.04407953392651729</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="U6">
-        <v>-0.04593332778983993</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="V6">
-        <v>-0.04765154737684933</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="W6">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="X6">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Y6">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Z6">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AA6">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AB6">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AC6">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AD6">
-        <v>-0.04361157366410478</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AE6">
-        <v>-0.02919886395325669</v>
+        <v>-0.1048858824530204</v>
       </c>
       <c r="AF6">
-        <v>-0.031750207957397</v>
+        <v>-0.1065406804703833</v>
       </c>
       <c r="AG6">
-        <v>-0.03400704503803546</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AH6">
-        <v>-0.036030384368919</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AI6">
-        <v>-0.03786883922263159</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AJ6">
-        <v>-0.03954496103361888</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AK6">
-        <v>-0.04108881936302056</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AL6">
-        <v>-0.04251977006019846</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AM6">
-        <v>-0.04361157366410478</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AN6">
-        <v>-0.04361157366410478</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AO6">
-        <v>-0.04361157366410478</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AP6">
-        <v>-0.04361157366410478</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AQ6">
-        <v>-0.04361157366410478</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AR6">
-        <v>-0.04361157366410478</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AS6">
-        <v>-0.04361157366410478</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AT6">
-        <v>0.2604262431281192</v>
+        <v>1.264613580403317</v>
       </c>
       <c r="AU6">
         <v>1</v>
@@ -5311,22 +5311,22 @@
         <v>243</v>
       </c>
       <c r="D7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E7">
-        <v>3892942</v>
+        <v>60209133</v>
       </c>
       <c r="F7">
-        <v>20</v>
+        <v>13</v>
       </c>
       <c r="G7" t="s">
         <v>121</v>
       </c>
       <c r="H7" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="I7" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J7">
         <v>1</v>
@@ -5335,115 +5335,115 @@
         <v>273</v>
       </c>
       <c r="L7">
-        <v>15</v>
+        <v>4.128767123287671</v>
       </c>
       <c r="M7" t="s">
         <v>274</v>
       </c>
       <c r="N7">
-        <v>-0.04896253477920987</v>
+        <v>-0.07661074219142525</v>
       </c>
       <c r="O7">
-        <v>-0.04896253477920987</v>
+        <v>-0.08170878970879146</v>
       </c>
       <c r="P7">
-        <v>-0.04896253477920987</v>
+        <v>-0.08590630865020346</v>
       </c>
       <c r="Q7">
-        <v>-0.04896253477920987</v>
+        <v>-0.08945758291073504</v>
       </c>
       <c r="R7">
-        <v>-0.04896253477920987</v>
+        <v>-0.09254207541109638</v>
       </c>
       <c r="S7">
-        <v>-0.04896253477920987</v>
+        <v>-0.09526836069494964</v>
       </c>
       <c r="T7">
-        <v>-0.04896253477920987</v>
+        <v>-0.09771740299229356</v>
       </c>
       <c r="U7">
-        <v>-0.04896253477920987</v>
+        <v>-0.09992940263313309</v>
       </c>
       <c r="V7">
-        <v>-0.04896253477920987</v>
+        <v>-0.1019510284301417</v>
       </c>
       <c r="W7">
-        <v>-0.04896253477920987</v>
+        <v>-0.1038124681427034</v>
       </c>
       <c r="X7">
-        <v>-0.04896253477920987</v>
+        <v>-0.1055418094650553</v>
       </c>
       <c r="Y7">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Z7">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AA7">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AB7">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AC7">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AD7">
-        <v>-0.04361157366410478</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AE7">
-        <v>-0.04361157366410478</v>
+        <v>-0.08170878970879146</v>
       </c>
       <c r="AF7">
-        <v>-0.04361157366410478</v>
+        <v>-0.08590630865020346</v>
       </c>
       <c r="AG7">
-        <v>-0.04361157366410478</v>
+        <v>-0.08945758291073504</v>
       </c>
       <c r="AH7">
-        <v>-0.04361157366410478</v>
+        <v>-0.09254207541109638</v>
       </c>
       <c r="AI7">
-        <v>-0.04361157366410478</v>
+        <v>-0.09526836069494964</v>
       </c>
       <c r="AJ7">
-        <v>-0.04361157366410478</v>
+        <v>-0.09771740299229356</v>
       </c>
       <c r="AK7">
-        <v>-0.04361157366410478</v>
+        <v>-0.09992940263313309</v>
       </c>
       <c r="AL7">
-        <v>-0.04361157366410478</v>
+        <v>-0.1019510284301417</v>
       </c>
       <c r="AM7">
-        <v>-0.04361157366410478</v>
+        <v>-0.1038124681427034</v>
       </c>
       <c r="AN7">
-        <v>-0.04361157366410478</v>
+        <v>-0.1055418094650553</v>
       </c>
       <c r="AO7">
-        <v>-0.04361157366410478</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AP7">
-        <v>-0.04361157366410478</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AQ7">
-        <v>-0.04361157366410478</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AR7">
-        <v>-0.04361157366410478</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AS7">
-        <v>-0.04361157366410478</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AT7">
-        <v>1.029665740199685</v>
+        <v>1.07856967152957</v>
       </c>
       <c r="AU7">
         <v>1</v>
       </c>
       <c r="AV7" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="8" spans="1:48">
@@ -5457,22 +5457,22 @@
         <v>244</v>
       </c>
       <c r="D8" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E8">
-        <v>457415</v>
+        <v>413560</v>
       </c>
       <c r="F8">
-        <v>4</v>
+        <v>15</v>
       </c>
       <c r="G8" t="s">
         <v>121</v>
       </c>
       <c r="H8" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I8" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J8">
         <v>1</v>
@@ -5484,112 +5484,112 @@
         <v>15</v>
       </c>
       <c r="M8" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="N8">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="O8">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="P8">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Q8">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="R8">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="S8">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="T8">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="U8">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="V8">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="W8">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="X8">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Y8">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Z8">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AA8">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AB8">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AC8">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AD8">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AE8">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AF8">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AG8">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AH8">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AI8">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AJ8">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AK8">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AL8">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AM8">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AN8">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AO8">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AP8">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AQ8">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AR8">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AS8">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AT8">
-        <v>0.2059331480399371</v>
+        <v>1.796083296781027</v>
       </c>
       <c r="AU8">
         <v>1</v>
       </c>
       <c r="AV8" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="9" spans="1:48">
@@ -5597,28 +5597,28 @@
         <v>121</v>
       </c>
       <c r="B9">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C9" t="s">
         <v>245</v>
       </c>
       <c r="D9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E9">
-        <v>1310176</v>
+        <v>60177677</v>
       </c>
       <c r="F9">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="G9" t="s">
         <v>121</v>
       </c>
       <c r="H9" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="I9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J9">
         <v>1</v>
@@ -5627,115 +5627,115 @@
         <v>273</v>
       </c>
       <c r="L9">
-        <v>15</v>
+        <v>5.515068493150685</v>
       </c>
       <c r="M9" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="N9">
-        <v>-0.04896253477920987</v>
+        <v>-0.08341573783132147</v>
       </c>
       <c r="O9">
-        <v>-0.04896253477920987</v>
+        <v>-0.08733256269963491</v>
       </c>
       <c r="P9">
-        <v>-0.04896253477920987</v>
+        <v>-0.09069755258004414</v>
       </c>
       <c r="Q9">
-        <v>-0.04896253477920987</v>
+        <v>-0.09363303651106913</v>
       </c>
       <c r="R9">
-        <v>-0.04896253477920987</v>
+        <v>-0.09624228885973561</v>
       </c>
       <c r="S9">
-        <v>-0.04896253477920987</v>
+        <v>-0.09859062220561614</v>
       </c>
       <c r="T9">
-        <v>-0.04896253477920987</v>
+        <v>-0.1007310985196402</v>
       </c>
       <c r="U9">
-        <v>-0.04896253477920987</v>
+        <v>-0.1026876795304324</v>
       </c>
       <c r="V9">
-        <v>-0.04896253477920987</v>
+        <v>-0.104493837747214</v>
       </c>
       <c r="W9">
-        <v>-0.04896253477920987</v>
+        <v>-0.1061710601891372</v>
       </c>
       <c r="X9">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Y9">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Z9">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AA9">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AB9">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AC9">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AD9">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AE9">
-        <v>-0.0361370479186777</v>
+        <v>-0.08733256269963491</v>
       </c>
       <c r="AF9">
-        <v>-0.0361370479186777</v>
+        <v>-0.09069755258004414</v>
       </c>
       <c r="AG9">
-        <v>-0.0361370479186777</v>
+        <v>-0.09363303651106913</v>
       </c>
       <c r="AH9">
-        <v>-0.0361370479186777</v>
+        <v>-0.09624228885973561</v>
       </c>
       <c r="AI9">
-        <v>-0.0361370479186777</v>
+        <v>-0.09859062220561614</v>
       </c>
       <c r="AJ9">
-        <v>-0.0361370479186777</v>
+        <v>-0.1007310985196402</v>
       </c>
       <c r="AK9">
-        <v>-0.0361370479186777</v>
+        <v>-0.1026876795304324</v>
       </c>
       <c r="AL9">
-        <v>-0.0361370479186777</v>
+        <v>-0.104493837747214</v>
       </c>
       <c r="AM9">
-        <v>-0.0361370479186777</v>
+        <v>-0.1061710601891372</v>
       </c>
       <c r="AN9">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AO9">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AP9">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AQ9">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AR9">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AS9">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AT9">
-        <v>0.5148328700998427</v>
+        <v>0.8190645109982641</v>
       </c>
       <c r="AU9">
         <v>1</v>
       </c>
       <c r="AV9" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="10" spans="1:48">
@@ -5743,28 +5743,28 @@
         <v>121</v>
       </c>
       <c r="B10">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="C10" t="s">
         <v>246</v>
       </c>
       <c r="D10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E10">
-        <v>406049</v>
+        <v>3892942</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>20</v>
       </c>
       <c r="G10" t="s">
         <v>121</v>
       </c>
       <c r="H10" t="s">
-        <v>266</v>
+        <v>268</v>
       </c>
       <c r="I10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J10">
         <v>1</v>
@@ -5773,115 +5773,115 @@
         <v>273</v>
       </c>
       <c r="L10">
-        <v>13.13698630136986</v>
+        <v>15</v>
       </c>
       <c r="M10" t="s">
-        <v>268</v>
+        <v>274</v>
       </c>
       <c r="N10">
-        <v>-0.04584525506024515</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="O10">
-        <v>-0.0475742486724006</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="P10">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Q10">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="R10">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="S10">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="T10">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="U10">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="V10">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="W10">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="X10">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Y10">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Z10">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AA10">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AB10">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AC10">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AD10">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AE10">
-        <v>-0.03457694473566745</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AF10">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AG10">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AH10">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AI10">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AJ10">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AK10">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AL10">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AM10">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AN10">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AO10">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AP10">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AQ10">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AR10">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AS10">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AT10">
-        <v>0.1441440876442106</v>
+        <v>2.394777729041369</v>
       </c>
       <c r="AU10">
         <v>1</v>
       </c>
       <c r="AV10" t="s">
-        <v>276</v>
+        <v>278</v>
       </c>
     </row>
     <row r="11" spans="1:48">
@@ -5895,22 +5895,22 @@
         <v>247</v>
       </c>
       <c r="D11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E11">
-        <v>4520541</v>
+        <v>457415</v>
       </c>
       <c r="F11">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="G11" t="s">
         <v>121</v>
       </c>
       <c r="H11" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J11">
         <v>1</v>
@@ -5922,112 +5922,112 @@
         <v>15</v>
       </c>
       <c r="M11" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="N11">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="O11">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="P11">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Q11">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="R11">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="S11">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="T11">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="U11">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="V11">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="W11">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="X11">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Y11">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Z11">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AA11">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AB11">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AC11">
-        <v>-0.04896253477920987</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AD11">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AE11">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AF11">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AG11">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AH11">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AI11">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AJ11">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AK11">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AL11">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AM11">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AN11">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AO11">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AP11">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AQ11">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AR11">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AS11">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AT11">
-        <v>0.9266991661797168</v>
+        <v>0.4789555458082739</v>
       </c>
       <c r="AU11">
         <v>1</v>
       </c>
       <c r="AV11" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="12" spans="1:48">
@@ -6044,136 +6044,136 @@
         <v>262</v>
       </c>
       <c r="E12">
-        <v>1395912</v>
+        <v>1310176</v>
       </c>
       <c r="F12">
-        <v>37</v>
+        <v>10</v>
       </c>
       <c r="G12" t="s">
         <v>121</v>
       </c>
       <c r="H12" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I12" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="J12">
         <v>1</v>
       </c>
       <c r="K12" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="L12">
-        <v>2</v>
+        <v>15</v>
       </c>
       <c r="M12" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="N12">
-        <v>0.01708602373512184</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="O12">
-        <v>0.00635166994959057</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="P12">
-        <v>-0.001241341582786389</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Q12">
-        <v>-0.007131996745594137</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="R12">
-        <v>-0.01194555604251909</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="S12">
-        <v>-0.0160260110156118</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="T12">
-        <v>-0.01955062082921017</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="U12">
-        <v>-0.02265981617948949</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="V12">
-        <v>-0.02544127599201792</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="W12">
-        <v>-0.02796412620390244</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="X12">
-        <v>-0.0302608626036002</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Y12">
-        <v>-0.03237377642723904</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Z12">
-        <v>-0.03433012458168842</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AA12">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AB12">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AC12">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AD12">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AE12">
-        <v>0.00635166994959057</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AF12">
-        <v>-0.001241341582786389</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AG12">
-        <v>-0.007131996745594137</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AH12">
-        <v>-0.01194555604251909</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AI12">
-        <v>-0.0160260110156118</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AJ12">
-        <v>-0.01955062082921017</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AK12">
-        <v>-0.02265981617948949</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AL12">
-        <v>-0.02544127599201792</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AM12">
-        <v>-0.02796412620390244</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AN12">
-        <v>-0.0302608626036002</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AO12">
-        <v>-0.03237377642723904</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AP12">
-        <v>-0.03433012458168842</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AQ12">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AR12">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AS12">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AT12">
-        <v>-0.6215628407495908</v>
+        <v>1.197388864520685</v>
       </c>
       <c r="AU12">
         <v>1</v>
       </c>
       <c r="AV12" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="13" spans="1:48">
@@ -6190,136 +6190,136 @@
         <v>262</v>
       </c>
       <c r="E13">
-        <v>3936370</v>
+        <v>406049</v>
       </c>
       <c r="F13">
-        <v>14</v>
+        <v>3</v>
       </c>
       <c r="G13" t="s">
         <v>121</v>
       </c>
       <c r="H13" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="I13" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
       <c r="J13">
         <v>1</v>
       </c>
       <c r="K13" t="s">
-        <v>268</v>
+        <v>273</v>
       </c>
       <c r="L13">
-        <v>1.983561643835617</v>
+        <v>12.47123287671233</v>
       </c>
       <c r="M13" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="N13">
-        <v>0.01730402805126439</v>
+        <v>-0.1025949144685768</v>
       </c>
       <c r="O13">
-        <v>0.006496673276419035</v>
+        <v>-0.1044079462797438</v>
       </c>
       <c r="P13">
-        <v>-0.00113263893402462</v>
+        <v>-0.1060955436746831</v>
       </c>
       <c r="Q13">
-        <v>-0.007045058522173721</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="R13">
-        <v>-0.01187312078770029</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="S13">
-        <v>-0.01596395607782092</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="T13">
-        <v>-0.01949632542186914</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="U13">
-        <v>-0.02261155543578863</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="V13">
-        <v>-0.02539784264755785</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="W13">
-        <v>-0.02792465216461943</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="X13">
-        <v>-0.03022467806866633</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Y13">
-        <v>-0.03234037531884198</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Z13">
-        <v>-0.03429910926731757</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AA13">
-        <v>-0.03612739694802918</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AB13">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AC13">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AD13">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AE13">
-        <v>0.006496673276419035</v>
+        <v>-0.1044079462797438</v>
       </c>
       <c r="AF13">
-        <v>-0.00113263893402462</v>
+        <v>-0.1060955436746831</v>
       </c>
       <c r="AG13">
-        <v>-0.007045058522173721</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AH13">
-        <v>-0.01187312078770029</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AI13">
-        <v>-0.01596395607782092</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AJ13">
-        <v>-0.01949632542186914</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AK13">
-        <v>-0.02261155543578863</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AL13">
-        <v>-0.02539784264755785</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AM13">
-        <v>-0.02792465216461943</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AN13">
-        <v>-0.03022467806866633</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AO13">
-        <v>-0.03234037531884198</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AP13">
-        <v>-0.03429910926731757</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AQ13">
-        <v>-0.03612739694802918</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AR13">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AS13">
-        <v>-0.0361370479186777</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AT13">
-        <v>-0.2381356861249876</v>
+        <v>0.3429719179978429</v>
       </c>
       <c r="AU13">
         <v>1</v>
       </c>
       <c r="AV13" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="14" spans="1:48">
@@ -6327,7 +6327,7 @@
         <v>121</v>
       </c>
       <c r="B14">
-        <v>25</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
         <v>250</v>
@@ -6336,136 +6336,136 @@
         <v>262</v>
       </c>
       <c r="E14">
-        <v>60058696</v>
+        <v>4520541</v>
       </c>
       <c r="F14">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="G14" t="s">
         <v>121</v>
       </c>
       <c r="H14" t="s">
+        <v>267</v>
+      </c>
+      <c r="I14" t="s">
+        <v>262</v>
+      </c>
+      <c r="J14">
+        <v>1</v>
+      </c>
+      <c r="K14" t="s">
+        <v>273</v>
+      </c>
+      <c r="L14">
+        <v>15</v>
+      </c>
+      <c r="M14" t="s">
         <v>269</v>
       </c>
-      <c r="I14" t="s">
-        <v>271</v>
-      </c>
-      <c r="J14">
-        <v>1</v>
-      </c>
-      <c r="K14" t="s">
-        <v>269</v>
-      </c>
-      <c r="L14">
-        <v>2.476712328767123</v>
-      </c>
-      <c r="M14" t="s">
-        <v>270</v>
-      </c>
       <c r="N14">
-        <v>0.006776342712931059</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="O14">
-        <v>0.003116452581044551</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="P14">
-        <v>0.0003966332443102114</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Q14">
-        <v>-0.001772801839107233</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="R14">
-        <v>-0.003577547895742814</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="S14">
-        <v>-0.005126693530755275</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="T14">
-        <v>-0.006477238347422185</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="U14">
-        <v>-0.007677094091887646</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="V14">
-        <v>-0.008756537472039319</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="W14">
-        <v>-0.009740116186092274</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="X14">
-        <v>-0.01063894869326409</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Y14">
-        <v>-0.01146848862779716</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="Z14">
-        <v>-0.01223865931043298</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AA14">
-        <v>-0.01261484408687026</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AB14">
-        <v>-0.01261484408687026</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AC14">
-        <v>-0.01261484408687026</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AD14">
-        <v>-0.02</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AE14">
-        <v>-0.02</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AF14">
-        <v>-0.02</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AG14">
-        <v>-0.02</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AH14">
-        <v>-0.02</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AI14">
-        <v>-0.02</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AJ14">
-        <v>-0.02</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AK14">
-        <v>-0.02</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AL14">
-        <v>-0.02</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AM14">
-        <v>-0.02</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AN14">
-        <v>-0.02</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AO14">
-        <v>-0.02</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AP14">
-        <v>-0.02</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AQ14">
-        <v>-0.02</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AR14">
-        <v>-0.02</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AS14">
-        <v>-0.02</v>
+        <v>-0.1069346504804038</v>
       </c>
       <c r="AT14">
-        <v>-0.127883926234053</v>
+        <v>2.155299956137232</v>
       </c>
       <c r="AU14">
         <v>1</v>
       </c>
       <c r="AV14" t="s">
-        <v>275</v>
+        <v>277</v>
       </c>
     </row>
     <row r="15" spans="1:48">
@@ -6482,16 +6482,16 @@
         <v>263</v>
       </c>
       <c r="E15">
-        <v>4565068</v>
+        <v>1395912</v>
       </c>
       <c r="F15">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="G15" t="s">
         <v>121</v>
       </c>
       <c r="H15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="I15" t="s">
         <v>271</v>
@@ -6500,118 +6500,118 @@
         <v>1</v>
       </c>
       <c r="K15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="L15">
-        <v>0.8849315068493151</v>
+        <v>1.334246575342466</v>
       </c>
       <c r="M15" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="N15">
-        <v>0.03862436956382281</v>
+        <v>-0.03280617195706982</v>
       </c>
       <c r="O15">
-        <v>0.01861287995795803</v>
+        <v>-0.04758050901879888</v>
       </c>
       <c r="P15">
-        <v>0.007383817691128558</v>
+        <v>-0.05702056829185893</v>
       </c>
       <c r="Q15">
-        <v>-0.0004708580233586113</v>
+        <v>-0.06394416954901511</v>
       </c>
       <c r="R15">
-        <v>-0.006517333184450295</v>
+        <v>-0.06942473044991739</v>
       </c>
       <c r="S15">
-        <v>-0.01144657646824946</v>
+        <v>-0.07396124965407982</v>
       </c>
       <c r="T15">
-        <v>-0.01558853348147737</v>
+        <v>-0.07784152266669329</v>
       </c>
       <c r="U15">
-        <v>-0.01916818820371855</v>
+        <v>-0.081215442719685</v>
       </c>
       <c r="V15">
-        <v>-0.02232012452088623</v>
+        <v>-0.08420681716884477</v>
       </c>
       <c r="W15">
-        <v>-0.02514304813429936</v>
+        <v>-0.08689362742882946</v>
       </c>
       <c r="X15">
-        <v>-0.02768656106108656</v>
+        <v>-0.0893385816550675</v>
       </c>
       <c r="Y15">
-        <v>-0.03000652371343666</v>
+        <v>-0.09157041575237897</v>
       </c>
       <c r="Z15">
-        <v>-0.03213907683631479</v>
+        <v>-0.09362828108290312</v>
       </c>
       <c r="AA15">
-        <v>-0.03411745716661802</v>
+        <v>-0.09553734870591413</v>
       </c>
       <c r="AB15">
-        <v>-0.03595307378016861</v>
+        <v>-0.09672139931377495</v>
       </c>
       <c r="AC15">
-        <v>-0.0361370479186777</v>
+        <v>-0.09672139931377495</v>
       </c>
       <c r="AD15">
-        <v>-0.0361370479186777</v>
+        <v>-0.09672139931377495</v>
       </c>
       <c r="AE15">
-        <v>0.01861287995795803</v>
+        <v>-0.04758050901879888</v>
       </c>
       <c r="AF15">
-        <v>0.007383817691128558</v>
+        <v>-0.05702056829185893</v>
       </c>
       <c r="AG15">
-        <v>-0.0004708580233586113</v>
+        <v>-0.06394416954901511</v>
       </c>
       <c r="AH15">
-        <v>-0.006517333184450295</v>
+        <v>-0.06942473044991739</v>
       </c>
       <c r="AI15">
-        <v>-0.01144657646824946</v>
+        <v>-0.07396124965407982</v>
       </c>
       <c r="AJ15">
-        <v>-0.01558853348147737</v>
+        <v>-0.07784152266669329</v>
       </c>
       <c r="AK15">
-        <v>-0.01916818820371855</v>
+        <v>-0.081215442719685</v>
       </c>
       <c r="AL15">
-        <v>-0.02232012452088623</v>
+        <v>-0.08420681716884477</v>
       </c>
       <c r="AM15">
-        <v>-0.02514304813429936</v>
+        <v>-0.08689362742882946</v>
       </c>
       <c r="AN15">
-        <v>-0.02768656106108656</v>
+        <v>-0.0893385816550675</v>
       </c>
       <c r="AO15">
-        <v>-0.03000652371343666</v>
+        <v>-0.09157041575237897</v>
       </c>
       <c r="AP15">
-        <v>-0.03213907683631479</v>
+        <v>-0.09362828108290312</v>
       </c>
       <c r="AQ15">
-        <v>-0.03411745716661802</v>
+        <v>-0.09553734870591413</v>
       </c>
       <c r="AR15">
-        <v>-0.03595307378016861</v>
+        <v>-0.09672139931377495</v>
       </c>
       <c r="AS15">
-        <v>-0.0361370479186777</v>
+        <v>-0.09672139931377495</v>
       </c>
       <c r="AT15">
-        <v>-0.5578200939966876</v>
+        <v>1.255000111888334</v>
       </c>
       <c r="AU15">
         <v>1</v>
       </c>
       <c r="AV15" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="16" spans="1:48">
@@ -6619,145 +6619,145 @@
         <v>121</v>
       </c>
       <c r="B16">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
         <v>252</v>
       </c>
       <c r="D16" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E16">
-        <v>345317</v>
+        <v>3936370</v>
       </c>
       <c r="F16">
-        <v>124</v>
+        <v>14</v>
       </c>
       <c r="G16" t="s">
         <v>121</v>
       </c>
       <c r="H16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I16" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="J16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L16">
-        <v>1.117808219178082</v>
+        <v>1.317808219178082</v>
       </c>
       <c r="M16" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N16">
-        <v>-0.02</v>
+        <v>-0.03247871272576161</v>
       </c>
       <c r="O16">
-        <v>-0.02</v>
+        <v>-0.04739383187172566</v>
       </c>
       <c r="P16">
-        <v>-0.02</v>
+        <v>-0.05689012503234533</v>
       </c>
       <c r="Q16">
-        <v>-0.02</v>
+        <v>-0.06384386041693474</v>
       </c>
       <c r="R16">
-        <v>-0.02</v>
+        <v>-0.06934324542991209</v>
       </c>
       <c r="S16">
-        <v>-0.02</v>
+        <v>-0.07389263998856904</v>
       </c>
       <c r="T16">
-        <v>-0.02</v>
+        <v>-0.07778229684284312</v>
       </c>
       <c r="U16">
-        <v>-0.02</v>
+        <v>-0.08116332555768535</v>
       </c>
       <c r="V16">
-        <v>-0.02</v>
+        <v>-0.08416028508451953</v>
       </c>
       <c r="W16">
-        <v>-0.02</v>
+        <v>-0.08685159924753491</v>
       </c>
       <c r="X16">
-        <v>-0.02</v>
+        <v>-0.08930027170437682</v>
       </c>
       <c r="Y16">
-        <v>-0.02</v>
+        <v>-0.09153521178487892</v>
       </c>
       <c r="Z16">
-        <v>-0.02</v>
+        <v>-0.09359571723283149</v>
       </c>
       <c r="AA16">
-        <v>-0.02</v>
+        <v>-0.09550705660813208</v>
       </c>
       <c r="AB16">
-        <v>-0.02</v>
+        <v>-0.09672139931377495</v>
       </c>
       <c r="AC16">
-        <v>-0.02</v>
+        <v>-0.09672139931377495</v>
       </c>
       <c r="AD16">
-        <v>-0.02</v>
+        <v>-0.09672139931377495</v>
       </c>
       <c r="AE16">
-        <v>-0.02</v>
+        <v>-0.04739383187172566</v>
       </c>
       <c r="AF16">
-        <v>-0.02</v>
+        <v>-0.05689012503234533</v>
       </c>
       <c r="AG16">
-        <v>-0.02</v>
+        <v>-0.06384386041693474</v>
       </c>
       <c r="AH16">
-        <v>-0.02</v>
+        <v>-0.06934324542991209</v>
       </c>
       <c r="AI16">
-        <v>-0.02</v>
+        <v>-0.07389263998856904</v>
       </c>
       <c r="AJ16">
-        <v>-0.02</v>
+        <v>-0.07778229684284312</v>
       </c>
       <c r="AK16">
-        <v>-0.02</v>
+        <v>-0.08116332555768535</v>
       </c>
       <c r="AL16">
-        <v>-0.02</v>
+        <v>-0.08416028508451953</v>
       </c>
       <c r="AM16">
-        <v>-0.02</v>
+        <v>-0.08685159924753491</v>
       </c>
       <c r="AN16">
-        <v>-0.02</v>
+        <v>-0.08930027170437682</v>
       </c>
       <c r="AO16">
-        <v>-0.02</v>
+        <v>-0.09153521178487892</v>
       </c>
       <c r="AP16">
-        <v>-0.02</v>
+        <v>-0.09359571723283149</v>
       </c>
       <c r="AQ16">
-        <v>-0.02</v>
+        <v>-0.09550705660813208</v>
       </c>
       <c r="AR16">
-        <v>-0.02</v>
+        <v>-0.09672139931377495</v>
       </c>
       <c r="AS16">
-        <v>-0.02</v>
+        <v>-0.09672139931377495</v>
       </c>
       <c r="AT16">
-        <v>2.530612244897959</v>
+        <v>0.4699658644634864</v>
       </c>
       <c r="AU16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV16" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="17" spans="1:48">
@@ -6765,19 +6765,19 @@
         <v>121</v>
       </c>
       <c r="B17">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
         <v>253</v>
       </c>
       <c r="D17" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="E17">
-        <v>941780</v>
+        <v>60058696</v>
       </c>
       <c r="F17">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="G17" t="s">
         <v>121</v>
@@ -6786,124 +6786,124 @@
         <v>270</v>
       </c>
       <c r="I17" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="J17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K17" t="s">
         <v>270</v>
       </c>
       <c r="L17">
-        <v>2.191780821917808</v>
+        <v>1.810958904109589</v>
       </c>
       <c r="M17" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="N17">
-        <v>-0.02</v>
+        <v>-0.05154082146998134</v>
       </c>
       <c r="O17">
-        <v>-0.02</v>
+        <v>-0.05627438495321831</v>
       </c>
       <c r="P17">
-        <v>-0.02</v>
+        <v>-0.05955886864580023</v>
       </c>
       <c r="Q17">
-        <v>-0.02</v>
+        <v>-0.06206595169839012</v>
       </c>
       <c r="R17">
-        <v>-0.02</v>
+        <v>-0.06409808395398359</v>
       </c>
       <c r="S17">
-        <v>-0.02</v>
+        <v>-0.06580687397840131</v>
       </c>
       <c r="T17">
-        <v>-0.02</v>
+        <v>-0.06728500673698438</v>
       </c>
       <c r="U17">
-        <v>-0.02</v>
+        <v>-0.06858113773839268</v>
       </c>
       <c r="V17">
-        <v>-0.02</v>
+        <v>-0.0697378617524738</v>
       </c>
       <c r="W17">
-        <v>-0.02</v>
+        <v>-0.0707822759969325</v>
       </c>
       <c r="X17">
-        <v>-0.02</v>
+        <v>-0.07173676822886385</v>
       </c>
       <c r="Y17">
-        <v>-0.02</v>
+        <v>-0.07261118622479279</v>
       </c>
       <c r="Z17">
-        <v>-0.02</v>
+        <v>-0.07341988890830831</v>
       </c>
       <c r="AA17">
-        <v>-0.02</v>
+        <v>-0.07417206701552739</v>
       </c>
       <c r="AB17">
-        <v>-0.02</v>
+        <v>-0.07430263986990944</v>
       </c>
       <c r="AC17">
-        <v>-0.02</v>
+        <v>-0.07430263986990944</v>
       </c>
       <c r="AD17">
-        <v>-0.02</v>
+        <v>-0.07430263986990944</v>
       </c>
       <c r="AE17">
-        <v>-0.02</v>
+        <v>-0.05627438495321831</v>
       </c>
       <c r="AF17">
-        <v>-0.02</v>
+        <v>-0.05955886864580023</v>
       </c>
       <c r="AG17">
-        <v>-0.02</v>
+        <v>-0.06206595169839012</v>
       </c>
       <c r="AH17">
-        <v>-0.02</v>
+        <v>-0.06409808395398359</v>
       </c>
       <c r="AI17">
-        <v>-0.02</v>
+        <v>-0.06580687397840131</v>
       </c>
       <c r="AJ17">
-        <v>-0.02</v>
+        <v>-0.06728500673698438</v>
       </c>
       <c r="AK17">
-        <v>-0.02</v>
+        <v>-0.06858113773839268</v>
       </c>
       <c r="AL17">
-        <v>-0.02</v>
+        <v>-0.0697378617524738</v>
       </c>
       <c r="AM17">
-        <v>-0.02</v>
+        <v>-0.0707822759969325</v>
       </c>
       <c r="AN17">
-        <v>-0.02</v>
+        <v>-0.07173676822886385</v>
       </c>
       <c r="AO17">
-        <v>-0.02</v>
+        <v>-0.07261118622479279</v>
       </c>
       <c r="AP17">
-        <v>-0.02</v>
+        <v>-0.07341988890830831</v>
       </c>
       <c r="AQ17">
-        <v>-0.02</v>
+        <v>-0.07417206701552739</v>
       </c>
       <c r="AR17">
-        <v>-0.02</v>
+        <v>-0.07430263986990944</v>
       </c>
       <c r="AS17">
-        <v>-0.02</v>
+        <v>-0.07430263986990944</v>
       </c>
       <c r="AT17">
-        <v>0.3673469387755102</v>
+        <v>1.032491044524855</v>
       </c>
       <c r="AU17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV17" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
     </row>
     <row r="18" spans="1:48">
@@ -6911,7 +6911,7 @@
         <v>121</v>
       </c>
       <c r="B18">
-        <v>38</v>
+        <v>13</v>
       </c>
       <c r="C18" t="s">
         <v>254</v>
@@ -6920,136 +6920,136 @@
         <v>264</v>
       </c>
       <c r="E18">
-        <v>941731</v>
+        <v>4565068</v>
       </c>
       <c r="F18">
-        <v>31</v>
+        <v>15</v>
       </c>
       <c r="G18" t="s">
         <v>121</v>
       </c>
       <c r="H18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="I18" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="J18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="K18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="L18">
-        <v>2.405479452054795</v>
+        <v>0.5</v>
       </c>
       <c r="M18" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="N18">
-        <v>-0.02</v>
+        <v>-0.006879769167127833</v>
       </c>
       <c r="O18">
-        <v>-0.02</v>
+        <v>-0.03042383379161122</v>
       </c>
       <c r="P18">
-        <v>-0.02</v>
+        <v>-0.04627777604339166</v>
       </c>
       <c r="Q18">
-        <v>-0.02</v>
+        <v>-0.05609364138287103</v>
       </c>
       <c r="R18">
-        <v>-0.02</v>
+        <v>-0.06323387216298698</v>
       </c>
       <c r="S18">
-        <v>-0.02</v>
+        <v>-0.06884898494427927</v>
       </c>
       <c r="T18">
-        <v>-0.02</v>
+        <v>-0.0734888257372564</v>
       </c>
       <c r="U18">
-        <v>-0.02</v>
+        <v>-0.07742412584502591</v>
       </c>
       <c r="V18">
-        <v>-0.02</v>
+        <v>-0.08084844453446981</v>
       </c>
       <c r="W18">
-        <v>-0.02</v>
+        <v>-0.08387935793753658</v>
       </c>
       <c r="X18">
-        <v>-0.02</v>
+        <v>-0.08660509306633835</v>
       </c>
       <c r="Y18">
-        <v>-0.02</v>
+        <v>-0.0890692378143129</v>
       </c>
       <c r="Z18">
-        <v>-0.02</v>
+        <v>-0.09132299697922586</v>
       </c>
       <c r="AA18">
-        <v>-0.02</v>
+        <v>-0.09339948656781831</v>
       </c>
       <c r="AB18">
-        <v>-0.02</v>
+        <v>-0.09532965697310994</v>
       </c>
       <c r="AC18">
-        <v>-0.02</v>
+        <v>-0.09672139931377495</v>
       </c>
       <c r="AD18">
-        <v>-0.02</v>
+        <v>-0.09672139931377495</v>
       </c>
       <c r="AE18">
-        <v>-0.02</v>
+        <v>-0.03042383379161122</v>
       </c>
       <c r="AF18">
-        <v>-0.02</v>
+        <v>-0.04627777604339166</v>
       </c>
       <c r="AG18">
-        <v>-0.02</v>
+        <v>-0.05609364138287103</v>
       </c>
       <c r="AH18">
-        <v>-0.02</v>
+        <v>-0.06323387216298698</v>
       </c>
       <c r="AI18">
-        <v>-0.02</v>
+        <v>-0.06884898494427927</v>
       </c>
       <c r="AJ18">
-        <v>-0.02</v>
+        <v>-0.0734888257372564</v>
       </c>
       <c r="AK18">
-        <v>-0.02</v>
+        <v>-0.07742412584502591</v>
       </c>
       <c r="AL18">
-        <v>-0.02</v>
+        <v>-0.08084844453446981</v>
       </c>
       <c r="AM18">
-        <v>-0.02</v>
+        <v>-0.08387935793753658</v>
       </c>
       <c r="AN18">
-        <v>-0.02</v>
+        <v>-0.08660509306633835</v>
       </c>
       <c r="AO18">
-        <v>-0.02</v>
+        <v>-0.0890692378143129</v>
       </c>
       <c r="AP18">
-        <v>-0.02</v>
+        <v>-0.09132299697922586</v>
       </c>
       <c r="AQ18">
-        <v>-0.02</v>
+        <v>-0.09339948656781831</v>
       </c>
       <c r="AR18">
-        <v>-0.02</v>
+        <v>-0.09532965697310994</v>
       </c>
       <c r="AS18">
-        <v>-0.02</v>
+        <v>-0.09672139931377495</v>
       </c>
       <c r="AT18">
-        <v>0.6326530612244898</v>
+        <v>0.1039114241186816</v>
       </c>
       <c r="AU18">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="AV18" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="19" spans="1:48">
@@ -7063,7 +7063,7 @@
         <v>255</v>
       </c>
       <c r="D19" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E19">
         <v>1218441</v>
@@ -7075,10 +7075,10 @@
         <v>128</v>
       </c>
       <c r="H19" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I19" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J19">
         <v>1</v>
@@ -7090,7 +7090,7 @@
         <v>13.38630136986301</v>
       </c>
       <c r="M19" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="N19">
         <v>-0.04628716665981197</v>
@@ -7141,52 +7141,52 @@
         <v>-0.04896253477920987</v>
       </c>
       <c r="AD19">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AE19">
-        <v>-0.03503863675043723</v>
+        <v>-0.04798509368362156</v>
       </c>
       <c r="AF19">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AG19">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AH19">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AI19">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AJ19">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AK19">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AL19">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AM19">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AN19">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AO19">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AP19">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AQ19">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AR19">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AS19">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AT19">
         <v>0.09706730378724263</v>
@@ -7195,7 +7195,7 @@
         <v>1</v>
       </c>
       <c r="AV19" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="20" spans="1:48">
@@ -7209,7 +7209,7 @@
         <v>256</v>
       </c>
       <c r="D20" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E20">
         <v>60055924</v>
@@ -7221,10 +7221,10 @@
         <v>128</v>
       </c>
       <c r="H20" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="I20" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J20">
         <v>1</v>
@@ -7287,52 +7287,52 @@
         <v>-0.04896253477920987</v>
       </c>
       <c r="AD20">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AE20">
-        <v>-0.03756930381072473</v>
+        <v>-0.04170725587089447</v>
       </c>
       <c r="AF20">
-        <v>-0.03927017866165177</v>
+        <v>-0.04374958793004801</v>
       </c>
       <c r="AG20">
-        <v>-0.04083501116334636</v>
+        <v>-0.04562856661191542</v>
       </c>
       <c r="AH20">
-        <v>-0.04228396114531983</v>
+        <v>-0.04736839890979524</v>
       </c>
       <c r="AI20">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AJ20">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AK20">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AL20">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AM20">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AN20">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AO20">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AP20">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AQ20">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AR20">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AS20">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AT20">
         <v>0.7395372742482074</v>
@@ -7341,7 +7341,7 @@
         <v>1</v>
       </c>
       <c r="AV20" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="21" spans="1:48">
@@ -7355,7 +7355,7 @@
         <v>257</v>
       </c>
       <c r="D21" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E21">
         <v>60144910</v>
@@ -7367,10 +7367,10 @@
         <v>128</v>
       </c>
       <c r="H21" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="I21" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J21">
         <v>1</v>
@@ -7382,7 +7382,7 @@
         <v>7.317808219178082</v>
       </c>
       <c r="M21" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="N21">
         <v>-0.006647356104413221</v>
@@ -7433,52 +7433,52 @@
         <v>-0.01509139912581338</v>
       </c>
       <c r="AD21">
-        <v>-0.02</v>
+        <v>-0.01509139912581338</v>
       </c>
       <c r="AE21">
-        <v>-0.02</v>
+        <v>-0.008158156386945684</v>
       </c>
       <c r="AF21">
-        <v>-0.02</v>
+        <v>-0.009493379801801163</v>
       </c>
       <c r="AG21">
-        <v>-0.02</v>
+        <v>-0.01069239212509018</v>
       </c>
       <c r="AH21">
-        <v>-0.02</v>
+        <v>-0.01178042952012766</v>
       </c>
       <c r="AI21">
-        <v>-0.02</v>
+        <v>-0.01277892143247003</v>
       </c>
       <c r="AJ21">
-        <v>-0.02</v>
+        <v>-0.01369684080868297</v>
       </c>
       <c r="AK21">
-        <v>-0.02</v>
+        <v>-0.01454829609654285</v>
       </c>
       <c r="AL21">
-        <v>-0.02</v>
+        <v>-0.01509139912581338</v>
       </c>
       <c r="AM21">
-        <v>-0.02</v>
+        <v>-0.01509139912581338</v>
       </c>
       <c r="AN21">
-        <v>-0.02</v>
+        <v>-0.01509139912581338</v>
       </c>
       <c r="AO21">
-        <v>-0.02</v>
+        <v>-0.01509139912581338</v>
       </c>
       <c r="AP21">
-        <v>-0.02</v>
+        <v>-0.01509139912581338</v>
       </c>
       <c r="AQ21">
-        <v>-0.02</v>
+        <v>-0.01509139912581338</v>
       </c>
       <c r="AR21">
-        <v>-0.02</v>
+        <v>-0.01509139912581338</v>
       </c>
       <c r="AS21">
-        <v>-0.02</v>
+        <v>-0.01509139912581338</v>
       </c>
       <c r="AT21">
         <v>0.2475980482608367</v>
@@ -7487,7 +7487,7 @@
         <v>1</v>
       </c>
       <c r="AV21" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
     </row>
     <row r="22" spans="1:48">
@@ -7501,7 +7501,7 @@
         <v>258</v>
       </c>
       <c r="D22" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E22">
         <v>496678</v>
@@ -7513,10 +7513,10 @@
         <v>122</v>
       </c>
       <c r="H22" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I22" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J22">
         <v>1</v>
@@ -7528,7 +7528,7 @@
         <v>14.62191780821918</v>
       </c>
       <c r="M22" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="N22">
         <v>-0.04836247008897316</v>
@@ -7579,52 +7579,52 @@
         <v>-0.04896253477920987</v>
       </c>
       <c r="AD22">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AE22">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AF22">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AG22">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AH22">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AI22">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AJ22">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AK22">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AL22">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AM22">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AN22">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AO22">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AP22">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AQ22">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AR22">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AS22">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AT22">
         <v>0.4573823720901941</v>
@@ -7633,7 +7633,7 @@
         <v>1</v>
       </c>
       <c r="AV22" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="23" spans="1:48">
@@ -7647,7 +7647,7 @@
         <v>259</v>
       </c>
       <c r="D23" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E23">
         <v>596771</v>
@@ -7659,10 +7659,10 @@
         <v>168</v>
       </c>
       <c r="H23" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="I23" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J23">
         <v>1</v>
@@ -7674,7 +7674,7 @@
         <v>13.88493150684931</v>
       </c>
       <c r="M23" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="N23">
         <v>-0.04714682046984989</v>
@@ -7725,52 +7725,52 @@
         <v>-0.04896253477920987</v>
       </c>
       <c r="AD23">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AE23">
-        <v>-0.03593849478630882</v>
+        <v>-0.0487858486740003</v>
       </c>
       <c r="AF23">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AG23">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AH23">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AI23">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AJ23">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AK23">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AL23">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AM23">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AN23">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AO23">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AP23">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AQ23">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AR23">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AS23">
-        <v>-0.0361370479186777</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AT23">
         <v>0.5442759034755772</v>
@@ -7779,7 +7779,7 @@
         <v>1</v>
       </c>
       <c r="AV23" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
     </row>
     <row r="24" spans="1:48">
@@ -7793,7 +7793,7 @@
         <v>260</v>
       </c>
       <c r="D24" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="E24">
         <v>60168413</v>
@@ -7805,10 +7805,10 @@
         <v>114</v>
       </c>
       <c r="H24" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="I24" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="J24">
         <v>1</v>
@@ -7871,52 +7871,52 @@
         <v>-0.04896253477920987</v>
       </c>
       <c r="AD24">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AE24">
-        <v>-0.02977996272458456</v>
+        <v>-0.03235417441917252</v>
       </c>
       <c r="AF24">
-        <v>-0.03226121692424899</v>
+        <v>-0.03533355000116906</v>
       </c>
       <c r="AG24">
-        <v>-0.03446305292590255</v>
+        <v>-0.03797741310063497</v>
       </c>
       <c r="AH24">
-        <v>-0.03644208084739651</v>
+        <v>-0.04035373853564519</v>
       </c>
       <c r="AI24">
-        <v>-0.03824398249710099</v>
+        <v>-0.04251737891437576</v>
       </c>
       <c r="AJ24">
-        <v>-0.03988958961583459</v>
+        <v>-0.04449334803022762</v>
       </c>
       <c r="AK24">
-        <v>-0.04140752415017635</v>
+        <v>-0.0463160137963143</v>
       </c>
       <c r="AL24">
-        <v>-0.04281617837210835</v>
+        <v>-0.04800746080439115</v>
       </c>
       <c r="AM24">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AN24">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AO24">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AP24">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AQ24">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AR24">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AS24">
-        <v>-0.04361157366410478</v>
+        <v>-0.04896253477920987</v>
       </c>
       <c r="AT24">
         <v>0.3277283878667971</v>
@@ -7925,7 +7925,7 @@
         <v>1</v>
       </c>
       <c r="AV24" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
   </sheetData>
@@ -7990,31 +7990,31 @@
         <v>17</v>
       </c>
       <c r="D2">
-        <v>8.263819500402901</v>
+        <v>7.598066075745367</v>
       </c>
       <c r="E2">
         <v>374</v>
       </c>
       <c r="F2">
-        <v>6.576248574594051</v>
+        <v>18.61096798750696</v>
       </c>
       <c r="G2">
-        <v>-3.690231932046194</v>
+        <v>8.084861234691942</v>
       </c>
       <c r="H2">
-        <v>10.01001410958476</v>
+        <v>23.56168519065077</v>
       </c>
       <c r="I2">
-        <v>-0.01727971359017978</v>
+        <v>-0.04740307710430334</v>
       </c>
       <c r="J2">
-        <v>0.009965256793790588</v>
+        <v>-0.02115985754726329</v>
       </c>
       <c r="K2">
-        <v>-0.02606706528941771</v>
+        <v>-0.05926548273723047</v>
       </c>
       <c r="L2">
-        <v>0.0360323220832083</v>
+        <v>0.03810562518996718</v>
       </c>
     </row>
     <row r="3" spans="1:12">
@@ -8025,31 +8025,31 @@
         <v>17</v>
       </c>
       <c r="D3">
-        <v>8.263819500402901</v>
+        <v>7.598066075745367</v>
       </c>
       <c r="E3">
         <v>374</v>
       </c>
       <c r="F3">
-        <v>6.576248574594051</v>
+        <v>18.61096798750696</v>
       </c>
       <c r="G3">
-        <v>-3.690231932046194</v>
+        <v>8.084861234691942</v>
       </c>
       <c r="H3">
-        <v>10.01001410958476</v>
+        <v>23.56168519065077</v>
       </c>
       <c r="I3">
-        <v>-0.01727971359017978</v>
+        <v>-0.04740307710430334</v>
       </c>
       <c r="J3">
-        <v>0.009965256793790588</v>
+        <v>-0.02115985754726329</v>
       </c>
       <c r="K3">
-        <v>-0.02606706528941771</v>
+        <v>-0.05926548273723047</v>
       </c>
       <c r="L3">
-        <v>0.00360323220832083</v>
+        <v>0.003810562518996718</v>
       </c>
     </row>
     <row r="4" spans="1:12">
@@ -8415,13 +8415,13 @@
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>278</v>
+        <v>275</v>
       </c>
       <c r="E2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="F2" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="G2">
         <v>0</v>
@@ -8462,10 +8462,10 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F3" t="s">
         <v>273</v>
@@ -8486,16 +8486,16 @@
         <v>10.5</v>
       </c>
       <c r="L3">
-        <v>0.030984668908323</v>
+        <v>-0.02698744679287091</v>
       </c>
       <c r="M3">
-        <v>-0.04057867427553811</v>
+        <v>-0.09855078997673201</v>
       </c>
       <c r="N3">
-        <v>-1.833261793707401</v>
+        <v>1.69189415793147</v>
       </c>
       <c r="O3">
-        <v>2.579991776750135</v>
+        <v>6.66881519417548</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -8509,13 +8509,13 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E4" t="s">
         <v>271</v>
       </c>
       <c r="F4" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="G4">
         <v>1</v>
@@ -8533,16 +8533,16 @@
         <v>10.5</v>
       </c>
       <c r="L4">
-        <v>0.05370458222796941</v>
+        <v>-0.006879769167127833</v>
       </c>
       <c r="M4">
-        <v>-0.02671558400461935</v>
+        <v>-0.0872999353997166</v>
       </c>
       <c r="N4">
-        <v>-3.363848356387926</v>
+        <v>0.4572102661221988</v>
       </c>
       <c r="O4">
-        <v>1.811627223581525</v>
+        <v>6.312912598406215</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -8556,10 +8556,10 @@
         <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E5" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F5" t="s">
         <v>273</v>
@@ -8580,16 +8580,16 @@
         <v>10.5</v>
       </c>
       <c r="L5">
-        <v>0.030984668908323</v>
+        <v>-0.02698744679287091</v>
       </c>
       <c r="M5">
-        <v>-0.04057867427553811</v>
+        <v>-0.09855078997673201</v>
       </c>
       <c r="N5">
-        <v>-1.262245825175587</v>
+        <v>1.164910731690521</v>
       </c>
       <c r="O5">
-        <v>1.776387780713208</v>
+        <v>4.591643248448691</v>
       </c>
     </row>
     <row r="6" spans="1:15">
@@ -8603,10 +8603,10 @@
         <v>1</v>
       </c>
       <c r="D6" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E6" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F6" t="s">
         <v>272</v>
@@ -8627,16 +8627,16 @@
         <v>10.5</v>
       </c>
       <c r="L6">
-        <v>0.02492292829285174</v>
+        <v>-0.03676486749018744</v>
       </c>
       <c r="M6">
-        <v>-0.01089519808621839</v>
+        <v>-0.07258299386925757</v>
       </c>
       <c r="N6">
-        <v>-0.3161194455340514</v>
+        <v>0.4961854704438616</v>
       </c>
       <c r="O6">
-        <v>0.1431977428951814</v>
+        <v>1.017426803760085</v>
       </c>
     </row>
     <row r="7" spans="1:15">
@@ -8650,13 +8650,13 @@
         <v>1</v>
       </c>
       <c r="D7" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E7" t="s">
         <v>271</v>
       </c>
       <c r="F7" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="G7">
         <v>1</v>
@@ -8674,16 +8674,16 @@
         <v>10.5</v>
       </c>
       <c r="L7">
-        <v>0.02400310468506598</v>
+        <v>-0.0376846910979732</v>
       </c>
       <c r="M7">
-        <v>-0.008774812662701914</v>
+        <v>-0.07046260844574109</v>
       </c>
       <c r="N7">
-        <v>-0.4453687561391871</v>
+        <v>0.7440483636059328</v>
       </c>
       <c r="O7">
-        <v>0.1681973407467538</v>
+        <v>1.44027510096234</v>
       </c>
     </row>
     <row r="8" spans="1:15">
@@ -8697,10 +8697,10 @@
         <v>1</v>
       </c>
       <c r="D8" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E8" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F8" t="s">
         <v>273</v>
@@ -8744,10 +8744,10 @@
         <v>1</v>
       </c>
       <c r="D9" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E9" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F9" t="s">
         <v>273</v>
@@ -8791,10 +8791,10 @@
         <v>1</v>
       </c>
       <c r="D10" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E10" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F10" t="s">
         <v>272</v>
@@ -8838,10 +8838,10 @@
         <v>1</v>
       </c>
       <c r="D11" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E11" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F11" t="s">
         <v>273</v>
@@ -8885,10 +8885,10 @@
         <v>1</v>
       </c>
       <c r="D12" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="E12" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F12" t="s">
         <v>273</v>
@@ -8932,10 +8932,10 @@
         <v>1</v>
       </c>
       <c r="D13" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="E13" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="F13" t="s">
         <v>273</v>

</xml_diff>